<commit_message>
updated wall mapping excel with startPosition for pacman and each ghost
</commit_message>
<xml_diff>
--- a/pacman-wall-mapping.xlsx
+++ b/pacman-wall-mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wesleyhall/development/PROJECTS/wdi-project-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DEE5540-BDE3-4145-A6A6-F8146011A609}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19973AA5-54E3-A94E-B85A-34DD478FA807}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-220" yWindow="460" windowWidth="24260" windowHeight="20540" xr2:uid="{1EA259AE-86C8-2D4F-8109-A100E6DB6DF0}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24260" windowHeight="20540" xr2:uid="{1EA259AE-86C8-2D4F-8109-A100E6DB6DF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Level 1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Level 4" sheetId="4" r:id="rId4"/>
     <sheet name="Level 5" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="4">
   <si>
     <t>21,22,23,27,28,29,30,31,32,36,37,38,41,45,47,48,51,52,54,58,61,63,64,65,67,68,71,72,74,75,76,78,81,83,96,98,101,103,105,106,107,108,111,112,113,114,116,118,121,123,125,134,136,138,141,143,145,147,148,149,150,151,152,154,156,158,161,163,169,170,176,178,185,187,189,190,192,194,205,207,212,214,221,223,227,228,229,230,231,232,236,238,241,243,245,247,248,249,250,251,252,254,256,258,261,263,265,274,276,278,281,283,285,286,287,288,291,292,293,294,296,298,301,303,316,318,321,323,324,325,327,328,331,332,334,335,336,338,341,345,347,348,351,352,354,358,361,362,363,367,368,369,370,371,372,376,377,378</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t>22,23,24,25,26,27,28,29,30,31,32,33,34,35,36,37,38,61,62,63,65,66,67,68,69,70,71,72,73,74,75,76,77,102,103,104,105,106,107,108,109,110,111,112,113,114,116,117,118,142,143,144,145,146,147,148,149,150,151,152,153,154,155,156,157,181,182,184,185,186,187,188,189,190,191,192,193,194,195,197,198,201,202,204,205,206,207,208,209,210,211,212,213,214,215,217,218,242,243,244,245,246,247,248,249,250,251,252,253,254,255,256,257,282,283,284,285,286,287,288,289,290,291,292,293,294,,296,297,296,298,321,322,323,325,326,327,328,329,330,331,332,333,334,335,336,337,362,363,364,365,366,367,368,369,370,371,372,373,374,375,376,377,378</t>
+  </si>
+  <si>
+    <t>#</t>
   </si>
 </sst>
 </file>
@@ -74,7 +77,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -93,6 +96,36 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF8AD8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -106,7 +139,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -120,12 +153,32 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF8AD8"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -437,7 +490,7 @@
   <dimension ref="B1:U22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="W11" sqref="W11"/>
+      <selection activeCell="H22" sqref="B22:H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -970,7 +1023,7 @@
       <c r="J10" s="1">
         <v>168</v>
       </c>
-      <c r="K10" s="1">
+      <c r="K10" s="6">
         <v>169</v>
       </c>
       <c r="L10" s="1">
@@ -1038,7 +1091,7 @@
       <c r="L11" s="3">
         <v>190</v>
       </c>
-      <c r="M11" s="1">
+      <c r="M11" s="7">
         <v>191</v>
       </c>
       <c r="N11" s="1">
@@ -1091,7 +1144,7 @@
       <c r="I12" s="1">
         <v>207</v>
       </c>
-      <c r="J12" s="1">
+      <c r="J12" s="9">
         <v>208</v>
       </c>
       <c r="K12" s="3">
@@ -1159,7 +1212,7 @@
       <c r="K13" s="1">
         <v>229</v>
       </c>
-      <c r="L13" s="1">
+      <c r="L13" s="8">
         <v>230</v>
       </c>
       <c r="M13" s="1">
@@ -1593,7 +1646,7 @@
       <c r="K20" s="1">
         <v>369</v>
       </c>
-      <c r="L20" s="1">
+      <c r="L20" s="5">
         <v>370</v>
       </c>
       <c r="M20" s="1">
@@ -1686,7 +1739,29 @@
         <v>399</v>
       </c>
     </row>
-    <row r="22" spans="2:21" ht="40" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="2:21" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1697,7 +1772,7 @@
   <dimension ref="B1:U22"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:H4"/>
+      <selection activeCell="B22" sqref="B22:I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1797,7 +1872,7 @@
       <c r="J3" s="1">
         <v>28</v>
       </c>
-      <c r="K3" s="1">
+      <c r="K3" s="5">
         <v>29</v>
       </c>
       <c r="L3" s="1">
@@ -2290,7 +2365,7 @@
       <c r="I11" s="1">
         <v>187</v>
       </c>
-      <c r="J11" s="1">
+      <c r="J11" s="6">
         <v>188</v>
       </c>
       <c r="K11" s="3">
@@ -2299,7 +2374,7 @@
       <c r="L11" s="3">
         <v>190</v>
       </c>
-      <c r="M11" s="1">
+      <c r="M11" s="8">
         <v>191</v>
       </c>
       <c r="N11" s="1">
@@ -2352,7 +2427,7 @@
       <c r="I12" s="1">
         <v>207</v>
       </c>
-      <c r="J12" s="1">
+      <c r="J12" s="7">
         <v>208</v>
       </c>
       <c r="K12" s="3">
@@ -2361,7 +2436,7 @@
       <c r="L12" s="3">
         <v>210</v>
       </c>
-      <c r="M12" s="1">
+      <c r="M12" s="9">
         <v>211</v>
       </c>
       <c r="N12" s="1">
@@ -2947,7 +3022,29 @@
         <v>399</v>
       </c>
     </row>
-    <row r="22" spans="2:21" ht="40" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="2:21" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2957,8 +3054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE33577D-AA93-3143-8505-98DD3BA3657B}">
   <dimension ref="B1:V22"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H22" sqref="B22:H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3587,7 +3684,7 @@
       <c r="S11" s="1">
         <v>197</v>
       </c>
-      <c r="T11" s="1">
+      <c r="T11" s="5">
         <v>198</v>
       </c>
       <c r="U11" s="4">
@@ -3619,16 +3716,16 @@
       <c r="I12" s="2">
         <v>207</v>
       </c>
-      <c r="J12" s="1">
+      <c r="J12" s="6">
         <v>208</v>
       </c>
-      <c r="K12" s="1">
+      <c r="K12" s="7">
         <v>209</v>
       </c>
-      <c r="L12" s="1">
+      <c r="L12" s="8">
         <v>210</v>
       </c>
-      <c r="M12" s="1">
+      <c r="M12" s="9">
         <v>211</v>
       </c>
       <c r="N12" s="2">
@@ -4214,7 +4311,29 @@
         <v>399</v>
       </c>
     </row>
-    <row r="22" spans="2:21" ht="40" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="2:21" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4225,7 +4344,7 @@
   <dimension ref="B1:V22"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="V3" sqref="V3"/>
+      <selection activeCell="B22" sqref="B22:H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4632,7 +4751,7 @@
       <c r="G8" s="3">
         <v>125</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="6">
         <v>126</v>
       </c>
       <c r="I8" s="1">
@@ -4653,7 +4772,7 @@
       <c r="N8" s="1">
         <v>132</v>
       </c>
-      <c r="O8" s="1">
+      <c r="O8" s="7">
         <v>133</v>
       </c>
       <c r="P8" s="3">
@@ -4865,7 +4984,7 @@
       <c r="B12" s="4">
         <v>200</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="5">
         <v>201</v>
       </c>
       <c r="D12" s="1">
@@ -5066,7 +5185,7 @@
       <c r="G15" s="3">
         <v>265</v>
       </c>
-      <c r="H15" s="1">
+      <c r="H15" s="9">
         <v>266</v>
       </c>
       <c r="I15" s="1">
@@ -5084,7 +5203,7 @@
       <c r="M15" s="1">
         <v>271</v>
       </c>
-      <c r="N15" s="1">
+      <c r="N15" s="8">
         <v>272</v>
       </c>
       <c r="O15" s="3">
@@ -5481,7 +5600,29 @@
         <v>399</v>
       </c>
     </row>
-    <row r="22" spans="2:21" ht="40" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="2:21" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5492,7 +5633,7 @@
   <dimension ref="B1:V22"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="V3" sqref="V3"/>
+      <selection activeCell="W18" sqref="W18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5571,7 +5712,7 @@
       <c r="B3" s="4">
         <v>20</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="5">
         <v>21</v>
       </c>
       <c r="D3" s="2">
@@ -6059,7 +6200,7 @@
       <c r="S10" s="1">
         <v>177</v>
       </c>
-      <c r="T10" s="1">
+      <c r="T10" s="8">
         <v>178</v>
       </c>
       <c r="U10" s="4">
@@ -6194,7 +6335,7 @@
       <c r="B13" s="4">
         <v>220</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="7">
         <v>221</v>
       </c>
       <c r="D13" s="1">
@@ -6369,7 +6510,7 @@
       <c r="S15" s="1">
         <v>277</v>
       </c>
-      <c r="T15" s="1">
+      <c r="T15" s="9">
         <v>278</v>
       </c>
       <c r="U15" s="4">
@@ -6628,7 +6769,7 @@
       <c r="B20" s="4">
         <v>360</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="6">
         <v>361</v>
       </c>
       <c r="D20" s="2">
@@ -6748,7 +6889,29 @@
         <v>399</v>
       </c>
     </row>
-    <row r="22" spans="2:21" ht="40" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="2:21" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated wall mapping excel with superfood locations
</commit_message>
<xml_diff>
--- a/pacman-wall-mapping.xlsx
+++ b/pacman-wall-mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wesleyhall/development/PROJECTS/wdi-project-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19973AA5-54E3-A94E-B85A-34DD478FA807}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC9D7BB-9C13-6447-9F8A-E4C946967011}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="24260" windowHeight="20540" xr2:uid="{1EA259AE-86C8-2D4F-8109-A100E6DB6DF0}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24260" windowHeight="20540" activeTab="4" xr2:uid="{1EA259AE-86C8-2D4F-8109-A100E6DB6DF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Level 1" sheetId="1" r:id="rId1"/>
@@ -77,7 +77,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -126,6 +126,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -139,7 +145,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -166,6 +172,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -489,8 +498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{888E5F92-0FDF-8647-8DCE-E19EF0F1C882}">
   <dimension ref="B1:U22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H22" sqref="B22:H22"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -627,7 +636,7 @@
       <c r="B4" s="4">
         <v>40</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="10">
         <v>41</v>
       </c>
       <c r="D4" s="2">
@@ -678,7 +687,7 @@
       <c r="S4" s="2">
         <v>57</v>
       </c>
-      <c r="T4" s="1">
+      <c r="T4" s="10">
         <v>58</v>
       </c>
       <c r="U4" s="4">
@@ -1557,7 +1566,7 @@
       <c r="B19" s="4">
         <v>340</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="10">
         <v>341</v>
       </c>
       <c r="D19" s="2">
@@ -1608,7 +1617,7 @@
       <c r="S19" s="2">
         <v>357</v>
       </c>
-      <c r="T19" s="1">
+      <c r="T19" s="10">
         <v>358</v>
       </c>
       <c r="U19" s="4">
@@ -1761,6 +1770,7 @@
       <c r="H22" s="9" t="s">
         <v>3</v>
       </c>
+      <c r="I22" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1772,7 +1782,7 @@
   <dimension ref="B1:U22"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22:I22"/>
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2229,7 +2239,7 @@
       <c r="E9" s="1">
         <v>143</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="10">
         <v>144</v>
       </c>
       <c r="G9" s="1">
@@ -2262,7 +2272,7 @@
       <c r="P9" s="1">
         <v>154</v>
       </c>
-      <c r="Q9" s="1">
+      <c r="Q9" s="10">
         <v>155</v>
       </c>
       <c r="R9" s="1">
@@ -2539,7 +2549,7 @@
       <c r="E14" s="1">
         <v>243</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14" s="10">
         <v>244</v>
       </c>
       <c r="G14" s="1">
@@ -2572,7 +2582,7 @@
       <c r="P14" s="1">
         <v>254</v>
       </c>
-      <c r="Q14" s="1">
+      <c r="Q14" s="10">
         <v>255</v>
       </c>
       <c r="R14" s="1">
@@ -3044,6 +3054,7 @@
       <c r="H22" s="9" t="s">
         <v>3</v>
       </c>
+      <c r="I22" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3052,10 +3063,1303 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE33577D-AA93-3143-8505-98DD3BA3657B}">
+  <dimension ref="A1:V22"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="21" width="7.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4">
+        <v>2</v>
+      </c>
+      <c r="E2" s="4">
+        <v>3</v>
+      </c>
+      <c r="F2" s="4">
+        <v>4</v>
+      </c>
+      <c r="G2" s="4">
+        <v>5</v>
+      </c>
+      <c r="H2" s="4">
+        <v>6</v>
+      </c>
+      <c r="I2" s="4">
+        <v>7</v>
+      </c>
+      <c r="J2" s="4">
+        <v>8</v>
+      </c>
+      <c r="K2" s="4">
+        <v>9</v>
+      </c>
+      <c r="L2" s="4">
+        <v>10</v>
+      </c>
+      <c r="M2" s="4">
+        <v>11</v>
+      </c>
+      <c r="N2" s="4">
+        <v>12</v>
+      </c>
+      <c r="O2" s="4">
+        <v>13</v>
+      </c>
+      <c r="P2" s="4">
+        <v>14</v>
+      </c>
+      <c r="Q2" s="4">
+        <v>15</v>
+      </c>
+      <c r="R2" s="4">
+        <v>16</v>
+      </c>
+      <c r="S2" s="4">
+        <v>17</v>
+      </c>
+      <c r="T2" s="4">
+        <v>18</v>
+      </c>
+      <c r="U2" s="4">
+        <v>19</v>
+      </c>
+      <c r="V2" t="str">
+        <f>C3&amp;","&amp;D3&amp;","&amp;E3&amp;","&amp;I3&amp;","&amp;J3&amp;","&amp;K3&amp;","&amp;L3&amp;","&amp;M3&amp;","&amp;N3&amp;","&amp;R3&amp;","&amp;S3&amp;","&amp;T3&amp;","&amp;C4&amp;","&amp;G4&amp;","&amp;I4&amp;","&amp;J4&amp;","&amp;M4&amp;","&amp;N4&amp;","&amp;P4&amp;","&amp;T4&amp;","&amp;C5&amp;","&amp;E5&amp;","&amp;F5&amp;","&amp;G5&amp;","&amp;I5&amp;","&amp;J5&amp;","&amp;M5&amp;","&amp;N5&amp;","&amp;P5&amp;","&amp;Q5&amp;","&amp;R5&amp;","&amp;T5&amp;","&amp;C6&amp;","&amp;E6&amp;","&amp;R6&amp;","&amp;T6&amp;","&amp;C7&amp;","&amp;E7&amp;","&amp;G7&amp;","&amp;H7&amp;","&amp;I7&amp;","&amp;J7&amp;","&amp;M7&amp;","&amp;N7&amp;","&amp;O7&amp;","&amp;P7&amp;","&amp;R7&amp;","&amp;T7&amp;","&amp;C8&amp;","&amp;E8&amp;","&amp;G8&amp;","&amp;P8&amp;","&amp;R8&amp;","&amp;T8&amp;","&amp;C9&amp;","&amp;E9&amp;","&amp;G9&amp;","&amp;I9&amp;","&amp;J9&amp;","&amp;K9&amp;","&amp;L9&amp;","&amp;M9&amp;","&amp;N9&amp;","&amp;P9&amp;","&amp;R9&amp;","&amp;T9&amp;","&amp;C10&amp;","&amp;E10&amp;","&amp;K10&amp;","&amp;L10&amp;","&amp;R10&amp;","&amp;T10&amp;","&amp;G11&amp;","&amp;I11&amp;","&amp;K11&amp;","&amp;L11&amp;","&amp;N11&amp;","&amp;P11&amp;","&amp;G12&amp;","&amp;I12&amp;","&amp;N12&amp;","&amp;P12&amp;","&amp;C13&amp;","&amp;E13&amp;","&amp;I13&amp;","&amp;J13&amp;","&amp;K13&amp;","&amp;L13&amp;","&amp;M13&amp;","&amp;N13&amp;","&amp;R13&amp;","&amp;T13&amp;","&amp;C14&amp;","&amp;E14&amp;","&amp;G14&amp;","&amp;I14&amp;","&amp;J14&amp;","&amp;K14&amp;","&amp;L14&amp;","&amp;M14&amp;","&amp;N14&amp;","&amp;P14&amp;","&amp;R14&amp;","&amp;T14&amp;","&amp;C15&amp;","&amp;E15&amp;","&amp;G15&amp;","&amp;P15&amp;","&amp;R15&amp;","&amp;T15&amp;","&amp;C16&amp;","&amp;E16&amp;","&amp;G16&amp;","&amp;H16&amp;","&amp;I16&amp;","&amp;J16&amp;","&amp;M16&amp;","&amp;N16&amp;","&amp;O16&amp;","&amp;P16&amp;","&amp;R16&amp;","&amp;T16&amp;","&amp;C17&amp;","&amp;E17&amp;","&amp;R17&amp;","&amp;T17&amp;","&amp;C18&amp;","&amp;E18&amp;","&amp;F18&amp;","&amp;G18&amp;","&amp;I18&amp;","&amp;J18&amp;","&amp;M18&amp;","&amp;N18&amp;","&amp;P18&amp;","&amp;Q18&amp;","&amp;R18&amp;","&amp;T18&amp;","&amp;C19&amp;","&amp;G19&amp;","&amp;I19&amp;","&amp;J19&amp;","&amp;M19&amp;","&amp;N19&amp;","&amp;P19&amp;","&amp;T19&amp;","&amp;C20&amp;","&amp;D20&amp;","&amp;E20&amp;","&amp;I20&amp;","&amp;J20&amp;","&amp;K20&amp;","&amp;L20&amp;","&amp;M20&amp;","&amp;N20&amp;","&amp;R20&amp;","&amp;S20&amp;","&amp;T20</f>
+        <v>21,22,23,27,28,29,30,31,32,36,37,38,41,45,47,48,51,52,54,58,61,63,64,65,67,68,71,72,74,75,76,78,81,83,96,98,101,103,105,106,107,108,111,112,113,114,116,118,121,123,125,134,136,138,141,143,145,147,148,149,150,151,152,154,156,158,161,163,169,170,176,178,185,187,189,190,192,194,205,207,212,214,221,223,227,228,229,230,231,232,236,238,241,243,245,247,248,249,250,251,252,254,256,258,261,263,265,274,276,278,281,283,285,286,287,288,291,292,293,294,296,298,301,303,316,318,321,323,324,325,327,328,331,332,334,335,336,338,341,345,347,348,351,352,354,358,361,362,363,367,368,369,370,371,372,376,377,378</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="4">
+        <v>20</v>
+      </c>
+      <c r="C3" s="2">
+        <v>21</v>
+      </c>
+      <c r="D3" s="2">
+        <v>22</v>
+      </c>
+      <c r="E3" s="2">
+        <v>23</v>
+      </c>
+      <c r="F3" s="1">
+        <v>24</v>
+      </c>
+      <c r="G3" s="1">
+        <v>25</v>
+      </c>
+      <c r="H3" s="1">
+        <v>26</v>
+      </c>
+      <c r="I3" s="2">
+        <v>27</v>
+      </c>
+      <c r="J3" s="2">
+        <v>28</v>
+      </c>
+      <c r="K3" s="2">
+        <v>29</v>
+      </c>
+      <c r="L3" s="2">
+        <v>30</v>
+      </c>
+      <c r="M3" s="2">
+        <v>31</v>
+      </c>
+      <c r="N3" s="2">
+        <v>32</v>
+      </c>
+      <c r="O3" s="1">
+        <v>33</v>
+      </c>
+      <c r="P3" s="1">
+        <v>34</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>35</v>
+      </c>
+      <c r="R3" s="2">
+        <v>36</v>
+      </c>
+      <c r="S3" s="2">
+        <v>37</v>
+      </c>
+      <c r="T3" s="2">
+        <v>38</v>
+      </c>
+      <c r="U3" s="4">
+        <v>39</v>
+      </c>
+      <c r="V3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="4">
+        <v>40</v>
+      </c>
+      <c r="C4" s="2">
+        <v>41</v>
+      </c>
+      <c r="D4" s="1">
+        <v>42</v>
+      </c>
+      <c r="E4" s="1">
+        <v>43</v>
+      </c>
+      <c r="F4" s="1">
+        <v>44</v>
+      </c>
+      <c r="G4" s="2">
+        <v>45</v>
+      </c>
+      <c r="H4" s="1">
+        <v>46</v>
+      </c>
+      <c r="I4" s="2">
+        <v>47</v>
+      </c>
+      <c r="J4" s="2">
+        <v>48</v>
+      </c>
+      <c r="K4" s="1">
+        <v>49</v>
+      </c>
+      <c r="L4" s="10">
+        <v>50</v>
+      </c>
+      <c r="M4" s="2">
+        <v>51</v>
+      </c>
+      <c r="N4" s="2">
+        <v>52</v>
+      </c>
+      <c r="O4" s="1">
+        <v>53</v>
+      </c>
+      <c r="P4" s="2">
+        <v>54</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>55</v>
+      </c>
+      <c r="R4" s="1">
+        <v>56</v>
+      </c>
+      <c r="S4" s="1">
+        <v>57</v>
+      </c>
+      <c r="T4" s="2">
+        <v>58</v>
+      </c>
+      <c r="U4" s="4">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="4">
+        <v>60</v>
+      </c>
+      <c r="C5" s="2">
+        <v>61</v>
+      </c>
+      <c r="D5" s="1">
+        <v>62</v>
+      </c>
+      <c r="E5" s="2">
+        <v>63</v>
+      </c>
+      <c r="F5" s="2">
+        <v>64</v>
+      </c>
+      <c r="G5" s="2">
+        <v>65</v>
+      </c>
+      <c r="H5" s="1">
+        <v>66</v>
+      </c>
+      <c r="I5" s="2">
+        <v>67</v>
+      </c>
+      <c r="J5" s="2">
+        <v>68</v>
+      </c>
+      <c r="K5" s="1">
+        <v>69</v>
+      </c>
+      <c r="L5" s="1">
+        <v>70</v>
+      </c>
+      <c r="M5" s="2">
+        <v>71</v>
+      </c>
+      <c r="N5" s="2">
+        <v>72</v>
+      </c>
+      <c r="O5" s="1">
+        <v>73</v>
+      </c>
+      <c r="P5" s="2">
+        <v>74</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>75</v>
+      </c>
+      <c r="R5" s="2">
+        <v>76</v>
+      </c>
+      <c r="S5" s="1">
+        <v>77</v>
+      </c>
+      <c r="T5" s="2">
+        <v>78</v>
+      </c>
+      <c r="U5" s="4">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="4">
+        <v>80</v>
+      </c>
+      <c r="C6" s="2">
+        <v>81</v>
+      </c>
+      <c r="D6" s="1">
+        <v>82</v>
+      </c>
+      <c r="E6" s="2">
+        <v>83</v>
+      </c>
+      <c r="F6" s="1">
+        <v>84</v>
+      </c>
+      <c r="G6" s="1">
+        <v>85</v>
+      </c>
+      <c r="H6" s="1">
+        <v>86</v>
+      </c>
+      <c r="I6" s="1">
+        <v>87</v>
+      </c>
+      <c r="J6" s="1">
+        <v>88</v>
+      </c>
+      <c r="K6" s="1">
+        <v>89</v>
+      </c>
+      <c r="L6" s="1">
+        <v>90</v>
+      </c>
+      <c r="M6" s="1">
+        <v>91</v>
+      </c>
+      <c r="N6" s="1">
+        <v>92</v>
+      </c>
+      <c r="O6" s="1">
+        <v>93</v>
+      </c>
+      <c r="P6" s="1">
+        <v>94</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>95</v>
+      </c>
+      <c r="R6" s="2">
+        <v>96</v>
+      </c>
+      <c r="S6" s="1">
+        <v>97</v>
+      </c>
+      <c r="T6" s="2">
+        <v>98</v>
+      </c>
+      <c r="U6" s="4">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="4">
+        <v>100</v>
+      </c>
+      <c r="C7" s="2">
+        <v>101</v>
+      </c>
+      <c r="D7" s="1">
+        <v>102</v>
+      </c>
+      <c r="E7" s="2">
+        <v>103</v>
+      </c>
+      <c r="F7" s="1">
+        <v>104</v>
+      </c>
+      <c r="G7" s="2">
+        <v>105</v>
+      </c>
+      <c r="H7" s="2">
+        <v>106</v>
+      </c>
+      <c r="I7" s="2">
+        <v>107</v>
+      </c>
+      <c r="J7" s="2">
+        <v>108</v>
+      </c>
+      <c r="K7" s="1">
+        <v>109</v>
+      </c>
+      <c r="L7" s="1">
+        <v>110</v>
+      </c>
+      <c r="M7" s="2">
+        <v>111</v>
+      </c>
+      <c r="N7" s="2">
+        <v>112</v>
+      </c>
+      <c r="O7" s="2">
+        <v>113</v>
+      </c>
+      <c r="P7" s="2">
+        <v>114</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>115</v>
+      </c>
+      <c r="R7" s="2">
+        <v>116</v>
+      </c>
+      <c r="S7" s="1">
+        <v>117</v>
+      </c>
+      <c r="T7" s="2">
+        <v>118</v>
+      </c>
+      <c r="U7" s="4">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="4">
+        <v>120</v>
+      </c>
+      <c r="C8" s="2">
+        <v>121</v>
+      </c>
+      <c r="D8" s="1">
+        <v>122</v>
+      </c>
+      <c r="E8" s="2">
+        <v>123</v>
+      </c>
+      <c r="F8" s="1">
+        <v>124</v>
+      </c>
+      <c r="G8" s="2">
+        <v>125</v>
+      </c>
+      <c r="H8" s="1">
+        <v>126</v>
+      </c>
+      <c r="I8" s="1">
+        <v>127</v>
+      </c>
+      <c r="J8" s="1">
+        <v>128</v>
+      </c>
+      <c r="K8" s="1">
+        <v>129</v>
+      </c>
+      <c r="L8" s="1">
+        <v>130</v>
+      </c>
+      <c r="M8" s="1">
+        <v>131</v>
+      </c>
+      <c r="N8" s="1">
+        <v>132</v>
+      </c>
+      <c r="O8" s="1">
+        <v>133</v>
+      </c>
+      <c r="P8" s="2">
+        <v>134</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>135</v>
+      </c>
+      <c r="R8" s="2">
+        <v>136</v>
+      </c>
+      <c r="S8" s="1">
+        <v>137</v>
+      </c>
+      <c r="T8" s="2">
+        <v>138</v>
+      </c>
+      <c r="U8" s="4">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="4">
+        <v>140</v>
+      </c>
+      <c r="C9" s="2">
+        <v>141</v>
+      </c>
+      <c r="D9" s="1">
+        <v>142</v>
+      </c>
+      <c r="E9" s="2">
+        <v>143</v>
+      </c>
+      <c r="F9" s="1">
+        <v>144</v>
+      </c>
+      <c r="G9" s="2">
+        <v>145</v>
+      </c>
+      <c r="H9" s="1">
+        <v>146</v>
+      </c>
+      <c r="I9" s="2">
+        <v>147</v>
+      </c>
+      <c r="J9" s="2">
+        <v>148</v>
+      </c>
+      <c r="K9" s="2">
+        <v>149</v>
+      </c>
+      <c r="L9" s="2">
+        <v>150</v>
+      </c>
+      <c r="M9" s="2">
+        <v>151</v>
+      </c>
+      <c r="N9" s="2">
+        <v>152</v>
+      </c>
+      <c r="O9" s="1">
+        <v>153</v>
+      </c>
+      <c r="P9" s="2">
+        <v>154</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>155</v>
+      </c>
+      <c r="R9" s="2">
+        <v>156</v>
+      </c>
+      <c r="S9" s="1">
+        <v>157</v>
+      </c>
+      <c r="T9" s="2">
+        <v>158</v>
+      </c>
+      <c r="U9" s="4">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="4">
+        <v>160</v>
+      </c>
+      <c r="C10" s="2">
+        <v>161</v>
+      </c>
+      <c r="D10" s="1">
+        <v>162</v>
+      </c>
+      <c r="E10" s="2">
+        <v>163</v>
+      </c>
+      <c r="F10" s="1">
+        <v>164</v>
+      </c>
+      <c r="G10" s="1">
+        <v>165</v>
+      </c>
+      <c r="H10" s="1">
+        <v>166</v>
+      </c>
+      <c r="I10" s="1">
+        <v>167</v>
+      </c>
+      <c r="J10" s="1">
+        <v>168</v>
+      </c>
+      <c r="K10" s="2">
+        <v>169</v>
+      </c>
+      <c r="L10" s="2">
+        <v>170</v>
+      </c>
+      <c r="M10" s="1">
+        <v>171</v>
+      </c>
+      <c r="N10" s="1">
+        <v>172</v>
+      </c>
+      <c r="O10" s="1">
+        <v>173</v>
+      </c>
+      <c r="P10" s="1">
+        <v>174</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>175</v>
+      </c>
+      <c r="R10" s="2">
+        <v>176</v>
+      </c>
+      <c r="S10" s="1">
+        <v>177</v>
+      </c>
+      <c r="T10" s="2">
+        <v>178</v>
+      </c>
+      <c r="U10" s="4">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="4">
+        <v>180</v>
+      </c>
+      <c r="C11" s="1">
+        <v>181</v>
+      </c>
+      <c r="D11" s="1">
+        <v>182</v>
+      </c>
+      <c r="E11" s="1">
+        <v>183</v>
+      </c>
+      <c r="F11" s="1">
+        <v>184</v>
+      </c>
+      <c r="G11" s="2">
+        <v>185</v>
+      </c>
+      <c r="H11" s="1">
+        <v>186</v>
+      </c>
+      <c r="I11" s="2">
+        <v>187</v>
+      </c>
+      <c r="J11" s="1">
+        <v>188</v>
+      </c>
+      <c r="K11" s="2">
+        <v>189</v>
+      </c>
+      <c r="L11" s="2">
+        <v>190</v>
+      </c>
+      <c r="M11" s="1">
+        <v>191</v>
+      </c>
+      <c r="N11" s="2">
+        <v>192</v>
+      </c>
+      <c r="O11" s="1">
+        <v>193</v>
+      </c>
+      <c r="P11" s="2">
+        <v>194</v>
+      </c>
+      <c r="Q11" s="10">
+        <v>195</v>
+      </c>
+      <c r="R11" s="1">
+        <v>196</v>
+      </c>
+      <c r="S11" s="1">
+        <v>197</v>
+      </c>
+      <c r="T11" s="5">
+        <v>198</v>
+      </c>
+      <c r="U11" s="4">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="4">
+        <v>200</v>
+      </c>
+      <c r="C12" s="1">
+        <v>201</v>
+      </c>
+      <c r="D12" s="1">
+        <v>202</v>
+      </c>
+      <c r="E12" s="1">
+        <v>203</v>
+      </c>
+      <c r="F12" s="10">
+        <v>204</v>
+      </c>
+      <c r="G12" s="2">
+        <v>205</v>
+      </c>
+      <c r="H12" s="1">
+        <v>206</v>
+      </c>
+      <c r="I12" s="2">
+        <v>207</v>
+      </c>
+      <c r="J12" s="6">
+        <v>208</v>
+      </c>
+      <c r="K12" s="7">
+        <v>209</v>
+      </c>
+      <c r="L12" s="8">
+        <v>210</v>
+      </c>
+      <c r="M12" s="9">
+        <v>211</v>
+      </c>
+      <c r="N12" s="2">
+        <v>212</v>
+      </c>
+      <c r="O12" s="1">
+        <v>213</v>
+      </c>
+      <c r="P12" s="2">
+        <v>214</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>215</v>
+      </c>
+      <c r="R12" s="1">
+        <v>216</v>
+      </c>
+      <c r="S12" s="1">
+        <v>217</v>
+      </c>
+      <c r="T12" s="1">
+        <v>218</v>
+      </c>
+      <c r="U12" s="4">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="4">
+        <v>220</v>
+      </c>
+      <c r="C13" s="2">
+        <v>221</v>
+      </c>
+      <c r="D13" s="1">
+        <v>222</v>
+      </c>
+      <c r="E13" s="2">
+        <v>223</v>
+      </c>
+      <c r="F13" s="1">
+        <v>224</v>
+      </c>
+      <c r="G13" s="1">
+        <v>225</v>
+      </c>
+      <c r="H13" s="1">
+        <v>226</v>
+      </c>
+      <c r="I13" s="2">
+        <v>227</v>
+      </c>
+      <c r="J13" s="2">
+        <v>228</v>
+      </c>
+      <c r="K13" s="2">
+        <v>229</v>
+      </c>
+      <c r="L13" s="2">
+        <v>230</v>
+      </c>
+      <c r="M13" s="2">
+        <v>231</v>
+      </c>
+      <c r="N13" s="2">
+        <v>232</v>
+      </c>
+      <c r="O13" s="1">
+        <v>233</v>
+      </c>
+      <c r="P13" s="1">
+        <v>234</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>235</v>
+      </c>
+      <c r="R13" s="2">
+        <v>236</v>
+      </c>
+      <c r="S13" s="1">
+        <v>237</v>
+      </c>
+      <c r="T13" s="2">
+        <v>238</v>
+      </c>
+      <c r="U13" s="4">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="4">
+        <v>240</v>
+      </c>
+      <c r="C14" s="2">
+        <v>241</v>
+      </c>
+      <c r="D14" s="1">
+        <v>242</v>
+      </c>
+      <c r="E14" s="2">
+        <v>243</v>
+      </c>
+      <c r="F14" s="1">
+        <v>244</v>
+      </c>
+      <c r="G14" s="2">
+        <v>245</v>
+      </c>
+      <c r="H14" s="1">
+        <v>246</v>
+      </c>
+      <c r="I14" s="2">
+        <v>247</v>
+      </c>
+      <c r="J14" s="2">
+        <v>248</v>
+      </c>
+      <c r="K14" s="2">
+        <v>249</v>
+      </c>
+      <c r="L14" s="2">
+        <v>250</v>
+      </c>
+      <c r="M14" s="2">
+        <v>251</v>
+      </c>
+      <c r="N14" s="2">
+        <v>252</v>
+      </c>
+      <c r="O14" s="1">
+        <v>253</v>
+      </c>
+      <c r="P14" s="2">
+        <v>254</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>255</v>
+      </c>
+      <c r="R14" s="2">
+        <v>256</v>
+      </c>
+      <c r="S14" s="1">
+        <v>257</v>
+      </c>
+      <c r="T14" s="2">
+        <v>258</v>
+      </c>
+      <c r="U14" s="4">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="4">
+        <v>260</v>
+      </c>
+      <c r="C15" s="2">
+        <v>261</v>
+      </c>
+      <c r="D15" s="1">
+        <v>262</v>
+      </c>
+      <c r="E15" s="2">
+        <v>263</v>
+      </c>
+      <c r="F15" s="1">
+        <v>264</v>
+      </c>
+      <c r="G15" s="2">
+        <v>265</v>
+      </c>
+      <c r="H15" s="1">
+        <v>266</v>
+      </c>
+      <c r="I15" s="1">
+        <v>267</v>
+      </c>
+      <c r="J15" s="1">
+        <v>268</v>
+      </c>
+      <c r="K15" s="1">
+        <v>269</v>
+      </c>
+      <c r="L15" s="1">
+        <v>270</v>
+      </c>
+      <c r="M15" s="1">
+        <v>271</v>
+      </c>
+      <c r="N15" s="1">
+        <v>272</v>
+      </c>
+      <c r="O15" s="1">
+        <v>273</v>
+      </c>
+      <c r="P15" s="2">
+        <v>274</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>275</v>
+      </c>
+      <c r="R15" s="2">
+        <v>276</v>
+      </c>
+      <c r="S15" s="1">
+        <v>277</v>
+      </c>
+      <c r="T15" s="2">
+        <v>278</v>
+      </c>
+      <c r="U15" s="4">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="4">
+        <v>280</v>
+      </c>
+      <c r="C16" s="2">
+        <v>281</v>
+      </c>
+      <c r="D16" s="1">
+        <v>282</v>
+      </c>
+      <c r="E16" s="2">
+        <v>283</v>
+      </c>
+      <c r="F16" s="1">
+        <v>284</v>
+      </c>
+      <c r="G16" s="2">
+        <v>285</v>
+      </c>
+      <c r="H16" s="2">
+        <v>286</v>
+      </c>
+      <c r="I16" s="2">
+        <v>287</v>
+      </c>
+      <c r="J16" s="2">
+        <v>288</v>
+      </c>
+      <c r="K16" s="1">
+        <v>289</v>
+      </c>
+      <c r="L16" s="1">
+        <v>290</v>
+      </c>
+      <c r="M16" s="2">
+        <v>291</v>
+      </c>
+      <c r="N16" s="2">
+        <v>292</v>
+      </c>
+      <c r="O16" s="2">
+        <v>293</v>
+      </c>
+      <c r="P16" s="2">
+        <v>294</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>295</v>
+      </c>
+      <c r="R16" s="2">
+        <v>296</v>
+      </c>
+      <c r="S16" s="1">
+        <v>297</v>
+      </c>
+      <c r="T16" s="2">
+        <v>298</v>
+      </c>
+      <c r="U16" s="4">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="17" spans="2:21" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="4">
+        <v>300</v>
+      </c>
+      <c r="C17" s="2">
+        <v>301</v>
+      </c>
+      <c r="D17" s="1">
+        <v>302</v>
+      </c>
+      <c r="E17" s="2">
+        <v>303</v>
+      </c>
+      <c r="F17" s="1">
+        <v>304</v>
+      </c>
+      <c r="G17" s="1">
+        <v>305</v>
+      </c>
+      <c r="H17" s="1">
+        <v>306</v>
+      </c>
+      <c r="I17" s="1">
+        <v>307</v>
+      </c>
+      <c r="J17" s="1">
+        <v>308</v>
+      </c>
+      <c r="K17" s="1">
+        <v>309</v>
+      </c>
+      <c r="L17" s="1">
+        <v>310</v>
+      </c>
+      <c r="M17" s="1">
+        <v>311</v>
+      </c>
+      <c r="N17" s="1">
+        <v>312</v>
+      </c>
+      <c r="O17" s="1">
+        <v>313</v>
+      </c>
+      <c r="P17" s="1">
+        <v>314</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>315</v>
+      </c>
+      <c r="R17" s="2">
+        <v>316</v>
+      </c>
+      <c r="S17" s="1">
+        <v>317</v>
+      </c>
+      <c r="T17" s="2">
+        <v>318</v>
+      </c>
+      <c r="U17" s="4">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="18" spans="2:21" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="4">
+        <v>320</v>
+      </c>
+      <c r="C18" s="2">
+        <v>321</v>
+      </c>
+      <c r="D18" s="1">
+        <v>322</v>
+      </c>
+      <c r="E18" s="2">
+        <v>323</v>
+      </c>
+      <c r="F18" s="2">
+        <v>324</v>
+      </c>
+      <c r="G18" s="2">
+        <v>325</v>
+      </c>
+      <c r="H18" s="1">
+        <v>326</v>
+      </c>
+      <c r="I18" s="2">
+        <v>327</v>
+      </c>
+      <c r="J18" s="2">
+        <v>328</v>
+      </c>
+      <c r="K18" s="1">
+        <v>329</v>
+      </c>
+      <c r="L18" s="1">
+        <v>330</v>
+      </c>
+      <c r="M18" s="2">
+        <v>331</v>
+      </c>
+      <c r="N18" s="2">
+        <v>332</v>
+      </c>
+      <c r="O18" s="1">
+        <v>333</v>
+      </c>
+      <c r="P18" s="2">
+        <v>334</v>
+      </c>
+      <c r="Q18" s="2">
+        <v>335</v>
+      </c>
+      <c r="R18" s="2">
+        <v>336</v>
+      </c>
+      <c r="S18" s="1">
+        <v>337</v>
+      </c>
+      <c r="T18" s="2">
+        <v>338</v>
+      </c>
+      <c r="U18" s="4">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="19" spans="2:21" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="4">
+        <v>340</v>
+      </c>
+      <c r="C19" s="2">
+        <v>341</v>
+      </c>
+      <c r="D19" s="1">
+        <v>342</v>
+      </c>
+      <c r="E19" s="1">
+        <v>343</v>
+      </c>
+      <c r="F19" s="1">
+        <v>344</v>
+      </c>
+      <c r="G19" s="2">
+        <v>345</v>
+      </c>
+      <c r="H19" s="1">
+        <v>346</v>
+      </c>
+      <c r="I19" s="2">
+        <v>347</v>
+      </c>
+      <c r="J19" s="2">
+        <v>348</v>
+      </c>
+      <c r="K19" s="10">
+        <v>349</v>
+      </c>
+      <c r="L19" s="1">
+        <v>350</v>
+      </c>
+      <c r="M19" s="2">
+        <v>351</v>
+      </c>
+      <c r="N19" s="2">
+        <v>352</v>
+      </c>
+      <c r="O19" s="1">
+        <v>353</v>
+      </c>
+      <c r="P19" s="2">
+        <v>354</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>355</v>
+      </c>
+      <c r="R19" s="1">
+        <v>356</v>
+      </c>
+      <c r="S19" s="1">
+        <v>357</v>
+      </c>
+      <c r="T19" s="2">
+        <v>358</v>
+      </c>
+      <c r="U19" s="4">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="20" spans="2:21" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="4">
+        <v>360</v>
+      </c>
+      <c r="C20" s="2">
+        <v>361</v>
+      </c>
+      <c r="D20" s="2">
+        <v>362</v>
+      </c>
+      <c r="E20" s="2">
+        <v>363</v>
+      </c>
+      <c r="F20" s="1">
+        <v>364</v>
+      </c>
+      <c r="G20" s="1">
+        <v>365</v>
+      </c>
+      <c r="H20" s="1">
+        <v>366</v>
+      </c>
+      <c r="I20" s="2">
+        <v>367</v>
+      </c>
+      <c r="J20" s="2">
+        <v>368</v>
+      </c>
+      <c r="K20" s="2">
+        <v>369</v>
+      </c>
+      <c r="L20" s="2">
+        <v>370</v>
+      </c>
+      <c r="M20" s="2">
+        <v>371</v>
+      </c>
+      <c r="N20" s="2">
+        <v>372</v>
+      </c>
+      <c r="O20" s="1">
+        <v>373</v>
+      </c>
+      <c r="P20" s="1">
+        <v>374</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>375</v>
+      </c>
+      <c r="R20" s="2">
+        <v>376</v>
+      </c>
+      <c r="S20" s="2">
+        <v>377</v>
+      </c>
+      <c r="T20" s="2">
+        <v>378</v>
+      </c>
+      <c r="U20" s="4">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="21" spans="2:21" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="4">
+        <v>380</v>
+      </c>
+      <c r="C21" s="4">
+        <v>381</v>
+      </c>
+      <c r="D21" s="4">
+        <v>382</v>
+      </c>
+      <c r="E21" s="4">
+        <v>383</v>
+      </c>
+      <c r="F21" s="4">
+        <v>384</v>
+      </c>
+      <c r="G21" s="4">
+        <v>385</v>
+      </c>
+      <c r="H21" s="4">
+        <v>386</v>
+      </c>
+      <c r="I21" s="4">
+        <v>387</v>
+      </c>
+      <c r="J21" s="4">
+        <v>388</v>
+      </c>
+      <c r="K21" s="4">
+        <v>389</v>
+      </c>
+      <c r="L21" s="4">
+        <v>390</v>
+      </c>
+      <c r="M21" s="4">
+        <v>391</v>
+      </c>
+      <c r="N21" s="4">
+        <v>392</v>
+      </c>
+      <c r="O21" s="4">
+        <v>393</v>
+      </c>
+      <c r="P21" s="4">
+        <v>394</v>
+      </c>
+      <c r="Q21" s="4">
+        <v>395</v>
+      </c>
+      <c r="R21" s="4">
+        <v>396</v>
+      </c>
+      <c r="S21" s="4">
+        <v>397</v>
+      </c>
+      <c r="T21" s="4">
+        <v>398</v>
+      </c>
+      <c r="U21" s="4">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="22" spans="2:21" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="I22" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51513D5F-F76C-D342-9541-5ACE88755250}">
   <dimension ref="B1:V22"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H22" sqref="B22:H22"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3126,8 +4430,8 @@
         <v>19</v>
       </c>
       <c r="V2" t="str">
-        <f>C3&amp;","&amp;D3&amp;","&amp;E3&amp;","&amp;I3&amp;","&amp;J3&amp;","&amp;K3&amp;","&amp;L3&amp;","&amp;M3&amp;","&amp;N3&amp;","&amp;R3&amp;","&amp;S3&amp;","&amp;T3&amp;","&amp;C4&amp;","&amp;G4&amp;","&amp;I4&amp;","&amp;J4&amp;","&amp;M4&amp;","&amp;N4&amp;","&amp;P4&amp;","&amp;T4&amp;","&amp;C5&amp;","&amp;E5&amp;","&amp;F5&amp;","&amp;G5&amp;","&amp;I5&amp;","&amp;J5&amp;","&amp;M5&amp;","&amp;N5&amp;","&amp;P5&amp;","&amp;Q5&amp;","&amp;R5&amp;","&amp;T5&amp;","&amp;C6&amp;","&amp;E6&amp;","&amp;R6&amp;","&amp;T6&amp;","&amp;C7&amp;","&amp;E7&amp;","&amp;G7&amp;","&amp;H7&amp;","&amp;I7&amp;","&amp;J7&amp;","&amp;M7&amp;","&amp;N7&amp;","&amp;O7&amp;","&amp;P7&amp;","&amp;R7&amp;","&amp;T7&amp;","&amp;C8&amp;","&amp;E8&amp;","&amp;G8&amp;","&amp;P8&amp;","&amp;R8&amp;","&amp;T8&amp;","&amp;C9&amp;","&amp;E9&amp;","&amp;G9&amp;","&amp;I9&amp;","&amp;J9&amp;","&amp;K9&amp;","&amp;L9&amp;","&amp;M9&amp;","&amp;N9&amp;","&amp;P9&amp;","&amp;R9&amp;","&amp;T9&amp;","&amp;C10&amp;","&amp;E10&amp;","&amp;K10&amp;","&amp;L10&amp;","&amp;R10&amp;","&amp;T10&amp;","&amp;G11&amp;","&amp;I11&amp;","&amp;K11&amp;","&amp;L11&amp;","&amp;N11&amp;","&amp;P11&amp;","&amp;G12&amp;","&amp;I12&amp;","&amp;N12&amp;","&amp;P12&amp;","&amp;C13&amp;","&amp;E13&amp;","&amp;I13&amp;","&amp;J13&amp;","&amp;K13&amp;","&amp;L13&amp;","&amp;M13&amp;","&amp;N13&amp;","&amp;R13&amp;","&amp;T13&amp;","&amp;C14&amp;","&amp;E14&amp;","&amp;G14&amp;","&amp;I14&amp;","&amp;J14&amp;","&amp;K14&amp;","&amp;L14&amp;","&amp;M14&amp;","&amp;N14&amp;","&amp;P14&amp;","&amp;R14&amp;","&amp;T14&amp;","&amp;C15&amp;","&amp;E15&amp;","&amp;G15&amp;","&amp;P15&amp;","&amp;R15&amp;","&amp;T15&amp;","&amp;C16&amp;","&amp;E16&amp;","&amp;G16&amp;","&amp;H16&amp;","&amp;I16&amp;","&amp;J16&amp;","&amp;M16&amp;","&amp;N16&amp;","&amp;O16&amp;","&amp;P16&amp;","&amp;R16&amp;","&amp;T16&amp;","&amp;C17&amp;","&amp;E17&amp;","&amp;R17&amp;","&amp;T17&amp;","&amp;C18&amp;","&amp;E18&amp;","&amp;F18&amp;","&amp;G18&amp;","&amp;I18&amp;","&amp;J18&amp;","&amp;M18&amp;","&amp;N18&amp;","&amp;P18&amp;","&amp;Q18&amp;","&amp;R18&amp;","&amp;T18&amp;","&amp;C19&amp;","&amp;G19&amp;","&amp;I19&amp;","&amp;J19&amp;","&amp;M19&amp;","&amp;N19&amp;","&amp;P19&amp;","&amp;T19&amp;","&amp;C20&amp;","&amp;D20&amp;","&amp;E20&amp;","&amp;I20&amp;","&amp;J20&amp;","&amp;K20&amp;","&amp;L20&amp;","&amp;M20&amp;","&amp;N20&amp;","&amp;R20&amp;","&amp;S20&amp;","&amp;T20</f>
-        <v>21,22,23,27,28,29,30,31,32,36,37,38,41,45,47,48,51,52,54,58,61,63,64,65,67,68,71,72,74,75,76,78,81,83,96,98,101,103,105,106,107,108,111,112,113,114,116,118,121,123,125,134,136,138,141,143,145,147,148,149,150,151,152,154,156,158,161,163,169,170,176,178,185,187,189,190,192,194,205,207,212,214,221,223,227,228,229,230,231,232,236,238,241,243,245,247,248,249,250,251,252,254,256,258,261,263,265,274,276,278,281,283,285,286,287,288,291,292,293,294,296,298,301,303,316,318,321,323,324,325,327,328,331,332,334,335,336,338,341,345,347,348,351,352,354,358,361,362,363,367,368,369,370,371,372,376,377,378</v>
+        <f>C3&amp;","&amp;D3&amp;","&amp;E3&amp;","&amp;F3&amp;","&amp;G3&amp;","&amp;H3&amp;","&amp;I3&amp;","&amp;J3&amp;","&amp;K3&amp;","&amp;L3&amp;","&amp;M3&amp;","&amp;N3&amp;","&amp;O3&amp;","&amp;P3&amp;","&amp;Q3&amp;","&amp;R3&amp;","&amp;S3&amp;","&amp;T3&amp;","&amp;C4&amp;","&amp;T4&amp;","&amp;C5&amp;","&amp;E5&amp;","&amp;F5&amp;","&amp;G5&amp;","&amp;H5&amp;","&amp;I5&amp;","&amp;J5&amp;","&amp;L5&amp;","&amp;M5&amp;","&amp;N5&amp;","&amp;O5&amp;","&amp;P5&amp;","&amp;Q5&amp;","&amp;R5&amp;","&amp;T5&amp;","&amp;C6&amp;","&amp;E6&amp;","&amp;R6&amp;","&amp;T6&amp;","&amp;C7&amp;","&amp;E7&amp;","&amp;G7&amp;","&amp;H7&amp;","&amp;I7&amp;","&amp;J7&amp;","&amp;K7&amp;","&amp;L7&amp;","&amp;M7&amp;","&amp;N7&amp;","&amp;O7&amp;","&amp;P7&amp;","&amp;R7&amp;","&amp;T7&amp;","&amp;C8&amp;","&amp;E8&amp;","&amp;G8&amp;","&amp;P8&amp;","&amp;R8&amp;","&amp;T8&amp;","&amp;C9&amp;","&amp;E9&amp;","&amp;G9&amp;","&amp;I9&amp;","&amp;J9&amp;","&amp;K9&amp;","&amp;M9&amp;","&amp;N9&amp;","&amp;P9&amp;","&amp;R9&amp;","&amp;T9&amp;","&amp;C10&amp;","&amp;E10&amp;","&amp;G10&amp;","&amp;I10&amp;","&amp;J10&amp;","&amp;K10&amp;","&amp;M10&amp;","&amp;N10&amp;","&amp;P10&amp;","&amp;R10&amp;","&amp;T10&amp;","&amp;C11&amp;","&amp;E11&amp;","&amp;G11&amp;","&amp;I11&amp;","&amp;J11&amp;","&amp;P11&amp;","&amp;R11&amp;","&amp;T11&amp;","&amp;E12&amp;","&amp;L12&amp;","&amp;M12&amp;","&amp;N12&amp;","&amp;P12&amp;","&amp;R12&amp;","&amp;T12&amp;","&amp;C13&amp;","&amp;E13&amp;","&amp;F13&amp;","&amp;G13&amp;","&amp;I13&amp;","&amp;J13&amp;","&amp;L13&amp;","&amp;M13&amp;","&amp;N13&amp;","&amp;P13&amp;","&amp;R13&amp;","&amp;T13&amp;","&amp;C14&amp;","&amp;G14&amp;","&amp;I14&amp;","&amp;J14&amp;","&amp;L14&amp;","&amp;M14&amp;","&amp;P14&amp;","&amp;R14&amp;","&amp;T14&amp;","&amp;C15&amp;","&amp;E15&amp;","&amp;G15&amp;","&amp;O15&amp;","&amp;P15&amp;","&amp;R15&amp;","&amp;T15&amp;","&amp;C16&amp;","&amp;E16&amp;","&amp;G16&amp;","&amp;H16&amp;","&amp;I16&amp;","&amp;J16&amp;","&amp;L16&amp;","&amp;M16&amp;","&amp;N16&amp;","&amp;O16&amp;","&amp;P16&amp;","&amp;R16&amp;","&amp;T16&amp;","&amp;C17&amp;","&amp;E17&amp;","&amp;R17&amp;","&amp;T17&amp;","&amp;C18&amp;","&amp;E18&amp;","&amp;F18&amp;","&amp;G18&amp;","&amp;H18&amp;","&amp;I18&amp;","&amp;J18&amp;","&amp;K18&amp;","&amp;L18&amp;","&amp;M18&amp;","&amp;N18&amp;","&amp;O18&amp;","&amp;P18&amp;","&amp;Q18&amp;","&amp;R18&amp;","&amp;T18&amp;","&amp;C19&amp;","&amp;T19&amp;","&amp;C20&amp;","&amp;D20&amp;","&amp;E20&amp;","&amp;F20&amp;","&amp;G20&amp;","&amp;H20&amp;","&amp;I20&amp;","&amp;J20&amp;","&amp;K20&amp;","&amp;L20&amp;","&amp;M20&amp;","&amp;N20&amp;","&amp;O20&amp;","&amp;P20&amp;","&amp;Q20&amp;","&amp;R20&amp;","&amp;S20&amp;","&amp;T20</f>
+        <v>21,22,23,24,25,26,27,28,29,30,31,32,33,34,35,36,37,38,41,58,61,63,64,65,66,67,68,70,71,72,73,74,75,76,78,81,83,96,98,101,103,105,106,107,108,109,110,111,112,113,114,116,118,121,123,125,134,136,138,141,143,145,147,148,149,151,152,154,156,158,161,163,165,167,168,169,171,172,174,176,178,181,183,185,187,188,194,196,198,203,210,211,212,214,216,218,221,223,224,225,227,228,230,231,232,234,236,238,241,245,247,248,250,251,254,256,258,261,263,265,273,274,276,278,281,283,285,286,287,288,290,291,292,293,294,296,298,301,303,316,318,321,323,324,325,326,327,328,329,330,331,332,333,334,335,336,338,341,358,361,362,363,364,365,366,367,368,369,370,371,372,373,374,375,376,377,378</v>
       </c>
     </row>
     <row r="3" spans="2:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -3143,13 +4447,13 @@
       <c r="E3" s="2">
         <v>23</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="2">
         <v>24</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="2">
         <v>25</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="2">
         <v>26</v>
       </c>
       <c r="I3" s="2">
@@ -3170,13 +4474,13 @@
       <c r="N3" s="2">
         <v>32</v>
       </c>
-      <c r="O3" s="1">
+      <c r="O3" s="2">
         <v>33</v>
       </c>
-      <c r="P3" s="1">
+      <c r="P3" s="2">
         <v>34</v>
       </c>
-      <c r="Q3" s="1">
+      <c r="Q3" s="2">
         <v>35</v>
       </c>
       <c r="R3" s="2">
@@ -3192,7 +4496,7 @@
         <v>39</v>
       </c>
       <c r="V3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="2:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
@@ -3211,16 +4515,16 @@
       <c r="F4" s="1">
         <v>44</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="1">
         <v>45</v>
       </c>
       <c r="H4" s="1">
         <v>46</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="1">
         <v>47</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="1">
         <v>48</v>
       </c>
       <c r="K4" s="1">
@@ -3229,16 +4533,16 @@
       <c r="L4" s="1">
         <v>50</v>
       </c>
-      <c r="M4" s="2">
+      <c r="M4" s="1">
         <v>51</v>
       </c>
-      <c r="N4" s="2">
+      <c r="N4" s="1">
         <v>52</v>
       </c>
       <c r="O4" s="1">
         <v>53</v>
       </c>
-      <c r="P4" s="2">
+      <c r="P4" s="1">
         <v>54</v>
       </c>
       <c r="Q4" s="1">
@@ -3276,7 +4580,7 @@
       <c r="G5" s="2">
         <v>65</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5" s="2">
         <v>66</v>
       </c>
       <c r="I5" s="2">
@@ -3285,10 +4589,10 @@
       <c r="J5" s="2">
         <v>68</v>
       </c>
-      <c r="K5" s="1">
+      <c r="K5" s="10">
         <v>69</v>
       </c>
-      <c r="L5" s="1">
+      <c r="L5" s="3">
         <v>70</v>
       </c>
       <c r="M5" s="2">
@@ -3297,7 +4601,7 @@
       <c r="N5" s="2">
         <v>72</v>
       </c>
-      <c r="O5" s="1">
+      <c r="O5" s="2">
         <v>73</v>
       </c>
       <c r="P5" s="2">
@@ -3397,34 +4701,34 @@
       <c r="F7" s="1">
         <v>104</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="3">
         <v>105</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="3">
         <v>106</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="3">
         <v>107</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J7" s="3">
         <v>108</v>
       </c>
-      <c r="K7" s="1">
+      <c r="K7" s="3">
         <v>109</v>
       </c>
-      <c r="L7" s="1">
+      <c r="L7" s="3">
         <v>110</v>
       </c>
-      <c r="M7" s="2">
+      <c r="M7" s="3">
         <v>111</v>
       </c>
-      <c r="N7" s="2">
+      <c r="N7" s="3">
         <v>112</v>
       </c>
-      <c r="O7" s="2">
+      <c r="O7" s="3">
         <v>113</v>
       </c>
-      <c r="P7" s="2">
+      <c r="P7" s="3">
         <v>114</v>
       </c>
       <c r="Q7" s="1">
@@ -3459,10 +4763,10 @@
       <c r="F8" s="1">
         <v>124</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="3">
         <v>125</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="6">
         <v>126</v>
       </c>
       <c r="I8" s="1">
@@ -3483,10 +4787,10 @@
       <c r="N8" s="1">
         <v>132</v>
       </c>
-      <c r="O8" s="1">
+      <c r="O8" s="7">
         <v>133</v>
       </c>
-      <c r="P8" s="2">
+      <c r="P8" s="3">
         <v>134</v>
       </c>
       <c r="Q8" s="1">
@@ -3521,34 +4825,34 @@
       <c r="F9" s="1">
         <v>144</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="3">
         <v>145</v>
       </c>
       <c r="H9" s="1">
         <v>146</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="3">
         <v>147</v>
       </c>
-      <c r="J9" s="2">
+      <c r="J9" s="3">
         <v>148</v>
       </c>
-      <c r="K9" s="2">
+      <c r="K9" s="3">
         <v>149</v>
       </c>
-      <c r="L9" s="2">
+      <c r="L9" s="1">
         <v>150</v>
       </c>
-      <c r="M9" s="2">
+      <c r="M9" s="3">
         <v>151</v>
       </c>
-      <c r="N9" s="2">
+      <c r="N9" s="3">
         <v>152</v>
       </c>
       <c r="O9" s="1">
         <v>153</v>
       </c>
-      <c r="P9" s="2">
+      <c r="P9" s="3">
         <v>154</v>
       </c>
       <c r="Q9" s="1">
@@ -3583,34 +4887,34 @@
       <c r="F10" s="1">
         <v>164</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="3">
         <v>165</v>
       </c>
       <c r="H10" s="1">
         <v>166</v>
       </c>
-      <c r="I10" s="1">
+      <c r="I10" s="3">
         <v>167</v>
       </c>
-      <c r="J10" s="1">
+      <c r="J10" s="3">
         <v>168</v>
       </c>
-      <c r="K10" s="2">
+      <c r="K10" s="3">
         <v>169</v>
       </c>
-      <c r="L10" s="2">
+      <c r="L10" s="1">
         <v>170</v>
       </c>
-      <c r="M10" s="1">
+      <c r="M10" s="3">
         <v>171</v>
       </c>
-      <c r="N10" s="1">
+      <c r="N10" s="3">
         <v>172</v>
       </c>
       <c r="O10" s="1">
         <v>173</v>
       </c>
-      <c r="P10" s="1">
+      <c r="P10" s="3">
         <v>174</v>
       </c>
       <c r="Q10" s="1">
@@ -3633,58 +4937,58 @@
       <c r="B11" s="4">
         <v>180</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="2">
         <v>181</v>
       </c>
       <c r="D11" s="1">
         <v>182</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="2">
         <v>183</v>
       </c>
       <c r="F11" s="1">
         <v>184</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="3">
         <v>185</v>
       </c>
       <c r="H11" s="1">
         <v>186</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11" s="3">
         <v>187</v>
       </c>
-      <c r="J11" s="1">
+      <c r="J11" s="3">
         <v>188</v>
       </c>
-      <c r="K11" s="2">
+      <c r="K11" s="1">
         <v>189</v>
       </c>
-      <c r="L11" s="2">
+      <c r="L11" s="1">
         <v>190</v>
       </c>
       <c r="M11" s="1">
         <v>191</v>
       </c>
-      <c r="N11" s="2">
+      <c r="N11" s="10">
         <v>192</v>
       </c>
       <c r="O11" s="1">
         <v>193</v>
       </c>
-      <c r="P11" s="2">
+      <c r="P11" s="3">
         <v>194</v>
       </c>
       <c r="Q11" s="1">
         <v>195</v>
       </c>
-      <c r="R11" s="1">
+      <c r="R11" s="2">
         <v>196</v>
       </c>
       <c r="S11" s="1">
         <v>197</v>
       </c>
-      <c r="T11" s="5">
+      <c r="T11" s="2">
         <v>198</v>
       </c>
       <c r="U11" s="4">
@@ -3695,58 +4999,58 @@
       <c r="B12" s="4">
         <v>200</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="5">
         <v>201</v>
       </c>
       <c r="D12" s="1">
         <v>202</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="3">
         <v>203</v>
       </c>
       <c r="F12" s="1">
         <v>204</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="1">
         <v>205</v>
       </c>
       <c r="H12" s="1">
         <v>206</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I12" s="10">
         <v>207</v>
       </c>
-      <c r="J12" s="6">
+      <c r="J12" s="1">
         <v>208</v>
       </c>
-      <c r="K12" s="7">
+      <c r="K12" s="1">
         <v>209</v>
       </c>
-      <c r="L12" s="8">
+      <c r="L12" s="3">
         <v>210</v>
       </c>
-      <c r="M12" s="9">
+      <c r="M12" s="3">
         <v>211</v>
       </c>
-      <c r="N12" s="2">
+      <c r="N12" s="3">
         <v>212</v>
       </c>
       <c r="O12" s="1">
         <v>213</v>
       </c>
-      <c r="P12" s="2">
+      <c r="P12" s="3">
         <v>214</v>
       </c>
       <c r="Q12" s="1">
         <v>215</v>
       </c>
-      <c r="R12" s="1">
+      <c r="R12" s="2">
         <v>216</v>
       </c>
       <c r="S12" s="1">
         <v>217</v>
       </c>
-      <c r="T12" s="1">
+      <c r="T12" s="2">
         <v>218</v>
       </c>
       <c r="U12" s="4">
@@ -3763,40 +5067,40 @@
       <c r="D13" s="1">
         <v>222</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="3">
         <v>223</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13" s="3">
         <v>224</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G13" s="3">
         <v>225</v>
       </c>
       <c r="H13" s="1">
         <v>226</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I13" s="3">
         <v>227</v>
       </c>
-      <c r="J13" s="2">
+      <c r="J13" s="3">
         <v>228</v>
       </c>
-      <c r="K13" s="2">
+      <c r="K13" s="1">
         <v>229</v>
       </c>
-      <c r="L13" s="2">
+      <c r="L13" s="3">
         <v>230</v>
       </c>
-      <c r="M13" s="2">
+      <c r="M13" s="3">
         <v>231</v>
       </c>
-      <c r="N13" s="2">
+      <c r="N13" s="3">
         <v>232</v>
       </c>
       <c r="O13" s="1">
         <v>233</v>
       </c>
-      <c r="P13" s="1">
+      <c r="P13" s="3">
         <v>234</v>
       </c>
       <c r="Q13" s="1">
@@ -3825,40 +5129,40 @@
       <c r="D14" s="1">
         <v>242</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="10">
         <v>243</v>
       </c>
       <c r="F14" s="1">
         <v>244</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14" s="3">
         <v>245</v>
       </c>
       <c r="H14" s="1">
         <v>246</v>
       </c>
-      <c r="I14" s="2">
+      <c r="I14" s="3">
         <v>247</v>
       </c>
-      <c r="J14" s="2">
+      <c r="J14" s="3">
         <v>248</v>
       </c>
-      <c r="K14" s="2">
+      <c r="K14" s="1">
         <v>249</v>
       </c>
-      <c r="L14" s="2">
+      <c r="L14" s="3">
         <v>250</v>
       </c>
-      <c r="M14" s="2">
+      <c r="M14" s="3">
         <v>251</v>
       </c>
-      <c r="N14" s="2">
+      <c r="N14" s="1">
         <v>252</v>
       </c>
       <c r="O14" s="1">
         <v>253</v>
       </c>
-      <c r="P14" s="2">
+      <c r="P14" s="3">
         <v>254</v>
       </c>
       <c r="Q14" s="1">
@@ -3893,10 +5197,10 @@
       <c r="F15" s="1">
         <v>264</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="3">
         <v>265</v>
       </c>
-      <c r="H15" s="1">
+      <c r="H15" s="9">
         <v>266</v>
       </c>
       <c r="I15" s="1">
@@ -3914,13 +5218,13 @@
       <c r="M15" s="1">
         <v>271</v>
       </c>
-      <c r="N15" s="1">
+      <c r="N15" s="8">
         <v>272</v>
       </c>
-      <c r="O15" s="1">
+      <c r="O15" s="3">
         <v>273</v>
       </c>
-      <c r="P15" s="2">
+      <c r="P15" s="3">
         <v>274</v>
       </c>
       <c r="Q15" s="1">
@@ -3955,34 +5259,34 @@
       <c r="F16" s="1">
         <v>284</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16" s="3">
         <v>285</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16" s="3">
         <v>286</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I16" s="3">
         <v>287</v>
       </c>
-      <c r="J16" s="2">
+      <c r="J16" s="3">
         <v>288</v>
       </c>
       <c r="K16" s="1">
         <v>289</v>
       </c>
-      <c r="L16" s="1">
+      <c r="L16" s="3">
         <v>290</v>
       </c>
-      <c r="M16" s="2">
+      <c r="M16" s="3">
         <v>291</v>
       </c>
-      <c r="N16" s="2">
+      <c r="N16" s="3">
         <v>292</v>
       </c>
-      <c r="O16" s="2">
+      <c r="O16" s="3">
         <v>293</v>
       </c>
-      <c r="P16" s="2">
+      <c r="P16" s="3">
         <v>294</v>
       </c>
       <c r="Q16" s="1">
@@ -4082,7 +5386,7 @@
       <c r="G18" s="2">
         <v>325</v>
       </c>
-      <c r="H18" s="1">
+      <c r="H18" s="2">
         <v>326</v>
       </c>
       <c r="I18" s="2">
@@ -4091,10 +5395,10 @@
       <c r="J18" s="2">
         <v>328</v>
       </c>
-      <c r="K18" s="1">
+      <c r="K18" s="2">
         <v>329</v>
       </c>
-      <c r="L18" s="1">
+      <c r="L18" s="2">
         <v>330</v>
       </c>
       <c r="M18" s="2">
@@ -4103,7 +5407,7 @@
       <c r="N18" s="2">
         <v>332</v>
       </c>
-      <c r="O18" s="1">
+      <c r="O18" s="2">
         <v>333</v>
       </c>
       <c r="P18" s="2">
@@ -4141,16 +5445,16 @@
       <c r="F19" s="1">
         <v>344</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G19" s="1">
         <v>345</v>
       </c>
       <c r="H19" s="1">
         <v>346</v>
       </c>
-      <c r="I19" s="2">
+      <c r="I19" s="1">
         <v>347</v>
       </c>
-      <c r="J19" s="2">
+      <c r="J19" s="1">
         <v>348</v>
       </c>
       <c r="K19" s="1">
@@ -4159,16 +5463,16 @@
       <c r="L19" s="1">
         <v>350</v>
       </c>
-      <c r="M19" s="2">
+      <c r="M19" s="1">
         <v>351</v>
       </c>
-      <c r="N19" s="2">
+      <c r="N19" s="1">
         <v>352</v>
       </c>
       <c r="O19" s="1">
         <v>353</v>
       </c>
-      <c r="P19" s="2">
+      <c r="P19" s="1">
         <v>354</v>
       </c>
       <c r="Q19" s="1">
@@ -4200,13 +5504,13 @@
       <c r="E20" s="2">
         <v>363</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F20" s="2">
         <v>364</v>
       </c>
-      <c r="G20" s="1">
+      <c r="G20" s="2">
         <v>365</v>
       </c>
-      <c r="H20" s="1">
+      <c r="H20" s="2">
         <v>366</v>
       </c>
       <c r="I20" s="2">
@@ -4227,13 +5531,13 @@
       <c r="N20" s="2">
         <v>372</v>
       </c>
-      <c r="O20" s="1">
+      <c r="O20" s="2">
         <v>373</v>
       </c>
-      <c r="P20" s="1">
+      <c r="P20" s="2">
         <v>374</v>
       </c>
-      <c r="Q20" s="1">
+      <c r="Q20" s="2">
         <v>375</v>
       </c>
       <c r="R20" s="2">
@@ -4333,18 +5637,19 @@
       <c r="H22" s="9" t="s">
         <v>3</v>
       </c>
+      <c r="I22" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51513D5F-F76C-D342-9541-5ACE88755250}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B86CBA31-09A1-CF47-B6B2-15E4927C6684}">
   <dimension ref="B1:V22"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22:H22"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4415,15 +5720,15 @@
         <v>19</v>
       </c>
       <c r="V2" t="str">
-        <f>C3&amp;","&amp;D3&amp;","&amp;E3&amp;","&amp;F3&amp;","&amp;G3&amp;","&amp;H3&amp;","&amp;I3&amp;","&amp;J3&amp;","&amp;K3&amp;","&amp;L3&amp;","&amp;M3&amp;","&amp;N3&amp;","&amp;O3&amp;","&amp;P3&amp;","&amp;Q3&amp;","&amp;R3&amp;","&amp;S3&amp;","&amp;T3&amp;","&amp;C4&amp;","&amp;T4&amp;","&amp;C5&amp;","&amp;E5&amp;","&amp;F5&amp;","&amp;G5&amp;","&amp;H5&amp;","&amp;I5&amp;","&amp;J5&amp;","&amp;L5&amp;","&amp;M5&amp;","&amp;N5&amp;","&amp;O5&amp;","&amp;P5&amp;","&amp;Q5&amp;","&amp;R5&amp;","&amp;T5&amp;","&amp;C6&amp;","&amp;E6&amp;","&amp;R6&amp;","&amp;T6&amp;","&amp;C7&amp;","&amp;E7&amp;","&amp;G7&amp;","&amp;H7&amp;","&amp;I7&amp;","&amp;J7&amp;","&amp;K7&amp;","&amp;L7&amp;","&amp;M7&amp;","&amp;N7&amp;","&amp;O7&amp;","&amp;P7&amp;","&amp;R7&amp;","&amp;T7&amp;","&amp;C8&amp;","&amp;E8&amp;","&amp;G8&amp;","&amp;P8&amp;","&amp;R8&amp;","&amp;T8&amp;","&amp;C9&amp;","&amp;E9&amp;","&amp;G9&amp;","&amp;I9&amp;","&amp;J9&amp;","&amp;K9&amp;","&amp;M9&amp;","&amp;N9&amp;","&amp;P9&amp;","&amp;R9&amp;","&amp;T9&amp;","&amp;C10&amp;","&amp;E10&amp;","&amp;G10&amp;","&amp;I10&amp;","&amp;J10&amp;","&amp;K10&amp;","&amp;M10&amp;","&amp;N10&amp;","&amp;P10&amp;","&amp;R10&amp;","&amp;T10&amp;","&amp;C11&amp;","&amp;E11&amp;","&amp;G11&amp;","&amp;I11&amp;","&amp;J11&amp;","&amp;P11&amp;","&amp;R11&amp;","&amp;T11&amp;","&amp;E12&amp;","&amp;L12&amp;","&amp;M12&amp;","&amp;N12&amp;","&amp;P12&amp;","&amp;R12&amp;","&amp;T12&amp;","&amp;C13&amp;","&amp;E13&amp;","&amp;F13&amp;","&amp;G13&amp;","&amp;I13&amp;","&amp;J13&amp;","&amp;L13&amp;","&amp;M13&amp;","&amp;N13&amp;","&amp;P13&amp;","&amp;R13&amp;","&amp;T13&amp;","&amp;C14&amp;","&amp;G14&amp;","&amp;I14&amp;","&amp;J14&amp;","&amp;L14&amp;","&amp;M14&amp;","&amp;P14&amp;","&amp;R14&amp;","&amp;T14&amp;","&amp;C15&amp;","&amp;E15&amp;","&amp;G15&amp;","&amp;O15&amp;","&amp;P15&amp;","&amp;R15&amp;","&amp;T15&amp;","&amp;C16&amp;","&amp;E16&amp;","&amp;G16&amp;","&amp;H16&amp;","&amp;I16&amp;","&amp;J16&amp;","&amp;L16&amp;","&amp;M16&amp;","&amp;N16&amp;","&amp;O16&amp;","&amp;P16&amp;","&amp;R16&amp;","&amp;T16&amp;","&amp;C17&amp;","&amp;E17&amp;","&amp;R17&amp;","&amp;T17&amp;","&amp;C18&amp;","&amp;E18&amp;","&amp;F18&amp;","&amp;G18&amp;","&amp;H18&amp;","&amp;I18&amp;","&amp;J18&amp;","&amp;K18&amp;","&amp;L18&amp;","&amp;M18&amp;","&amp;N18&amp;","&amp;O18&amp;","&amp;P18&amp;","&amp;Q18&amp;","&amp;R18&amp;","&amp;T18&amp;","&amp;C19&amp;","&amp;T19&amp;","&amp;C20&amp;","&amp;D20&amp;","&amp;E20&amp;","&amp;F20&amp;","&amp;G20&amp;","&amp;H20&amp;","&amp;I20&amp;","&amp;J20&amp;","&amp;K20&amp;","&amp;L20&amp;","&amp;M20&amp;","&amp;N20&amp;","&amp;O20&amp;","&amp;P20&amp;","&amp;Q20&amp;","&amp;R20&amp;","&amp;S20&amp;","&amp;T20</f>
-        <v>21,22,23,24,25,26,27,28,29,30,31,32,33,34,35,36,37,38,41,58,61,63,64,65,66,67,68,70,71,72,73,74,75,76,78,81,83,96,98,101,103,105,106,107,108,109,110,111,112,113,114,116,118,121,123,125,134,136,138,141,143,145,147,148,149,151,152,154,156,158,161,163,165,167,168,169,171,172,174,176,178,181,183,185,187,188,194,196,198,203,210,211,212,214,216,218,221,223,224,225,227,228,230,231,232,234,236,238,241,245,247,248,250,251,254,256,258,261,263,265,273,274,276,278,281,283,285,286,287,288,290,291,292,293,294,296,298,301,303,316,318,321,323,324,325,326,327,328,329,330,331,332,333,334,335,336,338,341,358,361,362,363,364,365,366,367,368,369,370,371,372,373,374,375,376,377,378</v>
+        <f>D3&amp;","&amp;E3&amp;","&amp;F3&amp;","&amp;G3&amp;","&amp;H3&amp;","&amp;I3&amp;","&amp;J3&amp;","&amp;K3&amp;","&amp;L3&amp;","&amp;M3&amp;","&amp;N3&amp;","&amp;O3&amp;","&amp;P3&amp;","&amp;Q3&amp;","&amp;R3&amp;","&amp;S3&amp;","&amp;T3&amp;","&amp;C5&amp;","&amp;D5&amp;","&amp;E5&amp;","&amp;G5&amp;","&amp;H5&amp;","&amp;I5&amp;","&amp;J5&amp;","&amp;K5&amp;","&amp;L5&amp;","&amp;M5&amp;","&amp;N5&amp;","&amp;O5&amp;","&amp;P5&amp;","&amp;Q5&amp;","&amp;R5&amp;","&amp;S5&amp;","&amp;D7&amp;","&amp;E7&amp;","&amp;F7&amp;","&amp;G7&amp;","&amp;H7&amp;","&amp;I7&amp;","&amp;J7&amp;","&amp;K7&amp;","&amp;L7&amp;","&amp;M7&amp;","&amp;N7&amp;","&amp;O7&amp;","&amp;P7&amp;","&amp;R7&amp;","&amp;S7&amp;","&amp;T7&amp;","&amp;D9&amp;","&amp;E9&amp;","&amp;F9&amp;","&amp;G9&amp;","&amp;H9&amp;","&amp;I9&amp;","&amp;J9&amp;","&amp;K9&amp;","&amp;L9&amp;","&amp;M9&amp;","&amp;N9&amp;","&amp;O9&amp;","&amp;P9&amp;","&amp;Q9&amp;","&amp;R9&amp;","&amp;S9&amp;","&amp;C11&amp;","&amp;D11&amp;","&amp;F11&amp;","&amp;G11&amp;","&amp;H11&amp;","&amp;I11&amp;","&amp;J11&amp;","&amp;K11&amp;","&amp;L11&amp;","&amp;M11&amp;","&amp;N11&amp;","&amp;O11&amp;","&amp;P11&amp;","&amp;Q11&amp;","&amp;S11&amp;","&amp;T11&amp;","&amp;C12&amp;","&amp;D12&amp;","&amp;F12&amp;","&amp;G12&amp;","&amp;H12&amp;","&amp;I12&amp;","&amp;J12&amp;","&amp;K12&amp;","&amp;L12&amp;","&amp;M12&amp;","&amp;N12&amp;","&amp;O12&amp;","&amp;P12&amp;","&amp;Q12&amp;","&amp;S12&amp;","&amp;T12&amp;","&amp;D14&amp;","&amp;E14&amp;","&amp;F14&amp;","&amp;G14&amp;","&amp;H14&amp;","&amp;I14&amp;","&amp;J14&amp;","&amp;K14&amp;","&amp;L14&amp;","&amp;M14&amp;","&amp;N14&amp;","&amp;O14&amp;","&amp;P14&amp;","&amp;Q14&amp;","&amp;R14&amp;","&amp;S14&amp;","&amp;D16&amp;","&amp;E16&amp;","&amp;F16&amp;","&amp;G16&amp;","&amp;H16&amp;","&amp;I16&amp;","&amp;J16&amp;","&amp;K16&amp;","&amp;L16&amp;","&amp;M16&amp;","&amp;N16&amp;","&amp;O16&amp;","&amp;P16&amp;","&amp;","&amp;R16&amp;","&amp;S16&amp;","&amp;R16&amp;","&amp;T16&amp;","&amp;C18&amp;","&amp;D18&amp;","&amp;E18&amp;","&amp;G18&amp;","&amp;H18&amp;","&amp;I18&amp;","&amp;J18&amp;","&amp;K18&amp;","&amp;L18&amp;","&amp;M18&amp;","&amp;N18&amp;","&amp;O18&amp;","&amp;P18&amp;","&amp;Q18&amp;","&amp;R18&amp;","&amp;S18&amp;","&amp;D20&amp;","&amp;E20&amp;","&amp;F20&amp;","&amp;G20&amp;","&amp;H20&amp;","&amp;I20&amp;","&amp;J20&amp;","&amp;K20&amp;","&amp;L20&amp;","&amp;M20&amp;","&amp;N20&amp;","&amp;O20&amp;","&amp;P20&amp;","&amp;Q20&amp;","&amp;R20&amp;","&amp;S20&amp;","&amp;T20</f>
+        <v>22,23,24,25,26,27,28,29,30,31,32,33,34,35,36,37,38,61,62,63,65,66,67,68,69,70,71,72,73,74,75,76,77,102,103,104,105,106,107,108,109,110,111,112,113,114,116,117,118,142,143,144,145,146,147,148,149,150,151,152,153,154,155,156,157,181,182,184,185,186,187,188,189,190,191,192,193,194,195,197,198,201,202,204,205,206,207,208,209,210,211,212,213,214,215,217,218,242,243,244,245,246,247,248,249,250,251,252,253,254,255,256,257,282,283,284,285,286,287,288,289,290,291,292,293,294,,296,297,296,298,321,322,323,325,326,327,328,329,330,331,332,333,334,335,336,337,362,363,364,365,366,367,368,369,370,371,372,373,374,375,376,377,378</v>
       </c>
     </row>
     <row r="3" spans="2:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="4">
         <v>20</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="5">
         <v>21</v>
       </c>
       <c r="D3" s="2">
@@ -4481,14 +5786,14 @@
         <v>39</v>
       </c>
       <c r="V3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="2:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="4">
         <v>40</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>41</v>
       </c>
       <c r="D4" s="1">
@@ -4539,7 +5844,7 @@
       <c r="S4" s="1">
         <v>57</v>
       </c>
-      <c r="T4" s="2">
+      <c r="T4" s="1">
         <v>58</v>
       </c>
       <c r="U4" s="4">
@@ -4553,13 +5858,13 @@
       <c r="C5" s="2">
         <v>61</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="2">
         <v>62</v>
       </c>
       <c r="E5" s="2">
         <v>63</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="10">
         <v>64</v>
       </c>
       <c r="G5" s="2">
@@ -4574,10 +5879,10 @@
       <c r="J5" s="2">
         <v>68</v>
       </c>
-      <c r="K5" s="1">
+      <c r="K5" s="2">
         <v>69</v>
       </c>
-      <c r="L5" s="3">
+      <c r="L5" s="2">
         <v>70</v>
       </c>
       <c r="M5" s="2">
@@ -4598,10 +5903,10 @@
       <c r="R5" s="2">
         <v>76</v>
       </c>
-      <c r="S5" s="1">
+      <c r="S5" s="2">
         <v>77</v>
       </c>
-      <c r="T5" s="2">
+      <c r="T5" s="1">
         <v>78</v>
       </c>
       <c r="U5" s="4">
@@ -4612,13 +5917,13 @@
       <c r="B6" s="4">
         <v>80</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>81</v>
       </c>
       <c r="D6" s="1">
         <v>82</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="1">
         <v>83</v>
       </c>
       <c r="F6" s="1">
@@ -4657,13 +5962,13 @@
       <c r="Q6" s="1">
         <v>95</v>
       </c>
-      <c r="R6" s="2">
+      <c r="R6" s="1">
         <v>96</v>
       </c>
       <c r="S6" s="1">
         <v>97</v>
       </c>
-      <c r="T6" s="2">
+      <c r="T6" s="1">
         <v>98</v>
       </c>
       <c r="U6" s="4">
@@ -4674,55 +5979,55 @@
       <c r="B7" s="4">
         <v>100</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>101</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="2">
         <v>102</v>
       </c>
       <c r="E7" s="2">
         <v>103</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="2">
         <v>104</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="2">
         <v>105</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="2">
         <v>106</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="2">
         <v>107</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7" s="2">
         <v>108</v>
       </c>
-      <c r="K7" s="3">
+      <c r="K7" s="2">
         <v>109</v>
       </c>
-      <c r="L7" s="3">
+      <c r="L7" s="2">
         <v>110</v>
       </c>
-      <c r="M7" s="3">
+      <c r="M7" s="2">
         <v>111</v>
       </c>
-      <c r="N7" s="3">
+      <c r="N7" s="2">
         <v>112</v>
       </c>
-      <c r="O7" s="3">
+      <c r="O7" s="2">
         <v>113</v>
       </c>
-      <c r="P7" s="3">
+      <c r="P7" s="2">
         <v>114</v>
       </c>
-      <c r="Q7" s="1">
+      <c r="Q7" s="10">
         <v>115</v>
       </c>
       <c r="R7" s="2">
         <v>116</v>
       </c>
-      <c r="S7" s="1">
+      <c r="S7" s="2">
         <v>117</v>
       </c>
       <c r="T7" s="2">
@@ -4736,22 +6041,22 @@
       <c r="B8" s="4">
         <v>120</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>121</v>
       </c>
       <c r="D8" s="1">
         <v>122</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="1">
         <v>123</v>
       </c>
       <c r="F8" s="1">
         <v>124</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="1">
         <v>125</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="1">
         <v>126</v>
       </c>
       <c r="I8" s="1">
@@ -4772,22 +6077,22 @@
       <c r="N8" s="1">
         <v>132</v>
       </c>
-      <c r="O8" s="7">
+      <c r="O8" s="1">
         <v>133</v>
       </c>
-      <c r="P8" s="3">
+      <c r="P8" s="1">
         <v>134</v>
       </c>
       <c r="Q8" s="1">
         <v>135</v>
       </c>
-      <c r="R8" s="2">
+      <c r="R8" s="1">
         <v>136</v>
       </c>
       <c r="S8" s="1">
         <v>137</v>
       </c>
-      <c r="T8" s="2">
+      <c r="T8" s="1">
         <v>138</v>
       </c>
       <c r="U8" s="4">
@@ -4798,58 +6103,58 @@
       <c r="B9" s="4">
         <v>140</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <v>141</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="2">
         <v>142</v>
       </c>
       <c r="E9" s="2">
         <v>143</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="2">
         <v>144</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="2">
         <v>145</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H9" s="2">
         <v>146</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9" s="2">
         <v>147</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J9" s="2">
         <v>148</v>
       </c>
-      <c r="K9" s="3">
+      <c r="K9" s="2">
         <v>149</v>
       </c>
-      <c r="L9" s="1">
+      <c r="L9" s="2">
         <v>150</v>
       </c>
-      <c r="M9" s="3">
+      <c r="M9" s="2">
         <v>151</v>
       </c>
-      <c r="N9" s="3">
+      <c r="N9" s="2">
         <v>152</v>
       </c>
-      <c r="O9" s="1">
+      <c r="O9" s="2">
         <v>153</v>
       </c>
-      <c r="P9" s="3">
+      <c r="P9" s="2">
         <v>154</v>
       </c>
-      <c r="Q9" s="1">
+      <c r="Q9" s="2">
         <v>155</v>
       </c>
       <c r="R9" s="2">
         <v>156</v>
       </c>
-      <c r="S9" s="1">
+      <c r="S9" s="2">
         <v>157</v>
       </c>
-      <c r="T9" s="2">
+      <c r="T9" s="1">
         <v>158</v>
       </c>
       <c r="U9" s="4">
@@ -4860,58 +6165,58 @@
       <c r="B10" s="4">
         <v>160</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="1">
         <v>161</v>
       </c>
       <c r="D10" s="1">
         <v>162</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="1">
         <v>163</v>
       </c>
       <c r="F10" s="1">
         <v>164</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="1">
         <v>165</v>
       </c>
       <c r="H10" s="1">
         <v>166</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I10" s="1">
         <v>167</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J10" s="1">
         <v>168</v>
       </c>
-      <c r="K10" s="3">
+      <c r="K10" s="1">
         <v>169</v>
       </c>
       <c r="L10" s="1">
         <v>170</v>
       </c>
-      <c r="M10" s="3">
+      <c r="M10" s="1">
         <v>171</v>
       </c>
-      <c r="N10" s="3">
+      <c r="N10" s="1">
         <v>172</v>
       </c>
       <c r="O10" s="1">
         <v>173</v>
       </c>
-      <c r="P10" s="3">
+      <c r="P10" s="1">
         <v>174</v>
       </c>
       <c r="Q10" s="1">
         <v>175</v>
       </c>
-      <c r="R10" s="2">
+      <c r="R10" s="1">
         <v>176</v>
       </c>
       <c r="S10" s="1">
         <v>177</v>
       </c>
-      <c r="T10" s="2">
+      <c r="T10" s="8">
         <v>178</v>
       </c>
       <c r="U10" s="4">
@@ -4925,52 +6230,52 @@
       <c r="C11" s="2">
         <v>181</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="2">
         <v>182</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="1">
         <v>183</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="2">
         <v>184</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="2">
         <v>185</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H11" s="2">
         <v>186</v>
       </c>
-      <c r="I11" s="3">
+      <c r="I11" s="2">
         <v>187</v>
       </c>
-      <c r="J11" s="3">
+      <c r="J11" s="2">
         <v>188</v>
       </c>
-      <c r="K11" s="1">
+      <c r="K11" s="2">
         <v>189</v>
       </c>
-      <c r="L11" s="1">
+      <c r="L11" s="2">
         <v>190</v>
       </c>
-      <c r="M11" s="1">
+      <c r="M11" s="2">
         <v>191</v>
       </c>
-      <c r="N11" s="1">
+      <c r="N11" s="2">
         <v>192</v>
       </c>
-      <c r="O11" s="1">
+      <c r="O11" s="2">
         <v>193</v>
       </c>
-      <c r="P11" s="3">
+      <c r="P11" s="2">
         <v>194</v>
       </c>
-      <c r="Q11" s="1">
+      <c r="Q11" s="2">
         <v>195</v>
       </c>
-      <c r="R11" s="2">
+      <c r="R11" s="1">
         <v>196</v>
       </c>
-      <c r="S11" s="1">
+      <c r="S11" s="2">
         <v>197</v>
       </c>
       <c r="T11" s="2">
@@ -4984,55 +6289,55 @@
       <c r="B12" s="4">
         <v>200</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="2">
         <v>201</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="2">
         <v>202</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="1">
         <v>203</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="2">
         <v>204</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12" s="2">
         <v>205</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H12" s="2">
         <v>206</v>
       </c>
-      <c r="I12" s="1">
+      <c r="I12" s="2">
         <v>207</v>
       </c>
-      <c r="J12" s="1">
+      <c r="J12" s="2">
         <v>208</v>
       </c>
-      <c r="K12" s="1">
+      <c r="K12" s="2">
         <v>209</v>
       </c>
-      <c r="L12" s="3">
+      <c r="L12" s="2">
         <v>210</v>
       </c>
-      <c r="M12" s="3">
+      <c r="M12" s="2">
         <v>211</v>
       </c>
-      <c r="N12" s="3">
+      <c r="N12" s="2">
         <v>212</v>
       </c>
-      <c r="O12" s="1">
+      <c r="O12" s="2">
         <v>213</v>
       </c>
-      <c r="P12" s="3">
+      <c r="P12" s="2">
         <v>214</v>
       </c>
-      <c r="Q12" s="1">
+      <c r="Q12" s="2">
         <v>215</v>
       </c>
-      <c r="R12" s="2">
+      <c r="R12" s="1">
         <v>216</v>
       </c>
-      <c r="S12" s="1">
+      <c r="S12" s="2">
         <v>217</v>
       </c>
       <c r="T12" s="2">
@@ -5046,58 +6351,58 @@
       <c r="B13" s="4">
         <v>220</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="7">
         <v>221</v>
       </c>
       <c r="D13" s="1">
         <v>222</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="1">
         <v>223</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="1">
         <v>224</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13" s="1">
         <v>225</v>
       </c>
       <c r="H13" s="1">
         <v>226</v>
       </c>
-      <c r="I13" s="3">
+      <c r="I13" s="1">
         <v>227</v>
       </c>
-      <c r="J13" s="3">
+      <c r="J13" s="1">
         <v>228</v>
       </c>
       <c r="K13" s="1">
         <v>229</v>
       </c>
-      <c r="L13" s="3">
+      <c r="L13" s="1">
         <v>230</v>
       </c>
-      <c r="M13" s="3">
+      <c r="M13" s="1">
         <v>231</v>
       </c>
-      <c r="N13" s="3">
+      <c r="N13" s="1">
         <v>232</v>
       </c>
       <c r="O13" s="1">
         <v>233</v>
       </c>
-      <c r="P13" s="3">
+      <c r="P13" s="1">
         <v>234</v>
       </c>
       <c r="Q13" s="1">
         <v>235</v>
       </c>
-      <c r="R13" s="2">
+      <c r="R13" s="1">
         <v>236</v>
       </c>
       <c r="S13" s="1">
         <v>237</v>
       </c>
-      <c r="T13" s="2">
+      <c r="T13" s="1">
         <v>238</v>
       </c>
       <c r="U13" s="4">
@@ -5108,58 +6413,58 @@
       <c r="B14" s="4">
         <v>240</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="1">
         <v>241</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="2">
         <v>242</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="2">
         <v>243</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14" s="2">
         <v>244</v>
       </c>
-      <c r="G14" s="3">
+      <c r="G14" s="2">
         <v>245</v>
       </c>
-      <c r="H14" s="1">
+      <c r="H14" s="2">
         <v>246</v>
       </c>
-      <c r="I14" s="3">
+      <c r="I14" s="2">
         <v>247</v>
       </c>
-      <c r="J14" s="3">
+      <c r="J14" s="2">
         <v>248</v>
       </c>
-      <c r="K14" s="1">
+      <c r="K14" s="2">
         <v>249</v>
       </c>
-      <c r="L14" s="3">
+      <c r="L14" s="2">
         <v>250</v>
       </c>
-      <c r="M14" s="3">
+      <c r="M14" s="2">
         <v>251</v>
       </c>
-      <c r="N14" s="1">
+      <c r="N14" s="2">
         <v>252</v>
       </c>
-      <c r="O14" s="1">
+      <c r="O14" s="2">
         <v>253</v>
       </c>
-      <c r="P14" s="3">
+      <c r="P14" s="2">
         <v>254</v>
       </c>
-      <c r="Q14" s="1">
+      <c r="Q14" s="2">
         <v>255</v>
       </c>
       <c r="R14" s="2">
         <v>256</v>
       </c>
-      <c r="S14" s="1">
+      <c r="S14" s="2">
         <v>257</v>
       </c>
-      <c r="T14" s="2">
+      <c r="T14" s="1">
         <v>258</v>
       </c>
       <c r="U14" s="4">
@@ -5170,22 +6475,22 @@
       <c r="B15" s="4">
         <v>260</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="1">
         <v>261</v>
       </c>
       <c r="D15" s="1">
         <v>262</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="1">
         <v>263</v>
       </c>
       <c r="F15" s="1">
         <v>264</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G15" s="1">
         <v>265</v>
       </c>
-      <c r="H15" s="9">
+      <c r="H15" s="1">
         <v>266</v>
       </c>
       <c r="I15" s="1">
@@ -5203,25 +6508,25 @@
       <c r="M15" s="1">
         <v>271</v>
       </c>
-      <c r="N15" s="8">
+      <c r="N15" s="1">
         <v>272</v>
       </c>
-      <c r="O15" s="3">
+      <c r="O15" s="1">
         <v>273</v>
       </c>
-      <c r="P15" s="3">
+      <c r="P15" s="1">
         <v>274</v>
       </c>
       <c r="Q15" s="1">
         <v>275</v>
       </c>
-      <c r="R15" s="2">
+      <c r="R15" s="1">
         <v>276</v>
       </c>
       <c r="S15" s="1">
         <v>277</v>
       </c>
-      <c r="T15" s="2">
+      <c r="T15" s="9">
         <v>278</v>
       </c>
       <c r="U15" s="4">
@@ -5232,55 +6537,55 @@
       <c r="B16" s="4">
         <v>280</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="1">
         <v>281</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="2">
         <v>282</v>
       </c>
       <c r="E16" s="2">
         <v>283</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16" s="2">
         <v>284</v>
       </c>
-      <c r="G16" s="3">
+      <c r="G16" s="2">
         <v>285</v>
       </c>
-      <c r="H16" s="3">
+      <c r="H16" s="2">
         <v>286</v>
       </c>
-      <c r="I16" s="3">
+      <c r="I16" s="2">
         <v>287</v>
       </c>
-      <c r="J16" s="3">
+      <c r="J16" s="2">
         <v>288</v>
       </c>
-      <c r="K16" s="1">
+      <c r="K16" s="2">
         <v>289</v>
       </c>
-      <c r="L16" s="3">
+      <c r="L16" s="2">
         <v>290</v>
       </c>
-      <c r="M16" s="3">
+      <c r="M16" s="2">
         <v>291</v>
       </c>
-      <c r="N16" s="3">
+      <c r="N16" s="2">
         <v>292</v>
       </c>
-      <c r="O16" s="3">
+      <c r="O16" s="2">
         <v>293</v>
       </c>
-      <c r="P16" s="3">
+      <c r="P16" s="2">
         <v>294</v>
       </c>
-      <c r="Q16" s="1">
+      <c r="Q16" s="10">
         <v>295</v>
       </c>
       <c r="R16" s="2">
         <v>296</v>
       </c>
-      <c r="S16" s="1">
+      <c r="S16" s="2">
         <v>297</v>
       </c>
       <c r="T16" s="2">
@@ -5294,13 +6599,13 @@
       <c r="B17" s="4">
         <v>300</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="1">
         <v>301</v>
       </c>
       <c r="D17" s="1">
         <v>302</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="1">
         <v>303</v>
       </c>
       <c r="F17" s="1">
@@ -5339,13 +6644,13 @@
       <c r="Q17" s="1">
         <v>315</v>
       </c>
-      <c r="R17" s="2">
+      <c r="R17" s="1">
         <v>316</v>
       </c>
       <c r="S17" s="1">
         <v>317</v>
       </c>
-      <c r="T17" s="2">
+      <c r="T17" s="1">
         <v>318</v>
       </c>
       <c r="U17" s="4">
@@ -5359,13 +6664,13 @@
       <c r="C18" s="2">
         <v>321</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18" s="2">
         <v>322</v>
       </c>
       <c r="E18" s="2">
         <v>323</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="10">
         <v>324</v>
       </c>
       <c r="G18" s="2">
@@ -5404,10 +6709,10 @@
       <c r="R18" s="2">
         <v>336</v>
       </c>
-      <c r="S18" s="1">
+      <c r="S18" s="2">
         <v>337</v>
       </c>
-      <c r="T18" s="2">
+      <c r="T18" s="1">
         <v>338</v>
       </c>
       <c r="U18" s="4">
@@ -5418,7 +6723,7 @@
       <c r="B19" s="4">
         <v>340</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="1">
         <v>341</v>
       </c>
       <c r="D19" s="1">
@@ -5469,7 +6774,7 @@
       <c r="S19" s="1">
         <v>357</v>
       </c>
-      <c r="T19" s="2">
+      <c r="T19" s="1">
         <v>358</v>
       </c>
       <c r="U19" s="4">
@@ -5480,7 +6785,7 @@
       <c r="B20" s="4">
         <v>360</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="6">
         <v>361</v>
       </c>
       <c r="D20" s="2">
@@ -5622,1295 +6927,7 @@
       <c r="H22" s="9" t="s">
         <v>3</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B86CBA31-09A1-CF47-B6B2-15E4927C6684}">
-  <dimension ref="B1:V22"/>
-  <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="W18" sqref="W18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="21" width="7.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:22" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="2:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="4">
-        <v>0</v>
-      </c>
-      <c r="C2" s="4">
-        <v>1</v>
-      </c>
-      <c r="D2" s="4">
-        <v>2</v>
-      </c>
-      <c r="E2" s="4">
-        <v>3</v>
-      </c>
-      <c r="F2" s="4">
-        <v>4</v>
-      </c>
-      <c r="G2" s="4">
-        <v>5</v>
-      </c>
-      <c r="H2" s="4">
-        <v>6</v>
-      </c>
-      <c r="I2" s="4">
-        <v>7</v>
-      </c>
-      <c r="J2" s="4">
-        <v>8</v>
-      </c>
-      <c r="K2" s="4">
-        <v>9</v>
-      </c>
-      <c r="L2" s="4">
-        <v>10</v>
-      </c>
-      <c r="M2" s="4">
-        <v>11</v>
-      </c>
-      <c r="N2" s="4">
-        <v>12</v>
-      </c>
-      <c r="O2" s="4">
-        <v>13</v>
-      </c>
-      <c r="P2" s="4">
-        <v>14</v>
-      </c>
-      <c r="Q2" s="4">
-        <v>15</v>
-      </c>
-      <c r="R2" s="4">
-        <v>16</v>
-      </c>
-      <c r="S2" s="4">
-        <v>17</v>
-      </c>
-      <c r="T2" s="4">
-        <v>18</v>
-      </c>
-      <c r="U2" s="4">
-        <v>19</v>
-      </c>
-      <c r="V2" t="str">
-        <f>D3&amp;","&amp;E3&amp;","&amp;F3&amp;","&amp;G3&amp;","&amp;H3&amp;","&amp;I3&amp;","&amp;J3&amp;","&amp;K3&amp;","&amp;L3&amp;","&amp;M3&amp;","&amp;N3&amp;","&amp;O3&amp;","&amp;P3&amp;","&amp;Q3&amp;","&amp;R3&amp;","&amp;S3&amp;","&amp;T3&amp;","&amp;C5&amp;","&amp;D5&amp;","&amp;E5&amp;","&amp;G5&amp;","&amp;H5&amp;","&amp;I5&amp;","&amp;J5&amp;","&amp;K5&amp;","&amp;L5&amp;","&amp;M5&amp;","&amp;N5&amp;","&amp;O5&amp;","&amp;P5&amp;","&amp;Q5&amp;","&amp;R5&amp;","&amp;S5&amp;","&amp;D7&amp;","&amp;E7&amp;","&amp;F7&amp;","&amp;G7&amp;","&amp;H7&amp;","&amp;I7&amp;","&amp;J7&amp;","&amp;K7&amp;","&amp;L7&amp;","&amp;M7&amp;","&amp;N7&amp;","&amp;O7&amp;","&amp;P7&amp;","&amp;R7&amp;","&amp;S7&amp;","&amp;T7&amp;","&amp;D9&amp;","&amp;E9&amp;","&amp;F9&amp;","&amp;G9&amp;","&amp;H9&amp;","&amp;I9&amp;","&amp;J9&amp;","&amp;K9&amp;","&amp;L9&amp;","&amp;M9&amp;","&amp;N9&amp;","&amp;O9&amp;","&amp;P9&amp;","&amp;Q9&amp;","&amp;R9&amp;","&amp;S9&amp;","&amp;C11&amp;","&amp;D11&amp;","&amp;F11&amp;","&amp;G11&amp;","&amp;H11&amp;","&amp;I11&amp;","&amp;J11&amp;","&amp;K11&amp;","&amp;L11&amp;","&amp;M11&amp;","&amp;N11&amp;","&amp;O11&amp;","&amp;P11&amp;","&amp;Q11&amp;","&amp;S11&amp;","&amp;T11&amp;","&amp;C12&amp;","&amp;D12&amp;","&amp;F12&amp;","&amp;G12&amp;","&amp;H12&amp;","&amp;I12&amp;","&amp;J12&amp;","&amp;K12&amp;","&amp;L12&amp;","&amp;M12&amp;","&amp;N12&amp;","&amp;O12&amp;","&amp;P12&amp;","&amp;Q12&amp;","&amp;S12&amp;","&amp;T12&amp;","&amp;D14&amp;","&amp;E14&amp;","&amp;F14&amp;","&amp;G14&amp;","&amp;H14&amp;","&amp;I14&amp;","&amp;J14&amp;","&amp;K14&amp;","&amp;L14&amp;","&amp;M14&amp;","&amp;N14&amp;","&amp;O14&amp;","&amp;P14&amp;","&amp;Q14&amp;","&amp;R14&amp;","&amp;S14&amp;","&amp;D16&amp;","&amp;E16&amp;","&amp;F16&amp;","&amp;G16&amp;","&amp;H16&amp;","&amp;I16&amp;","&amp;J16&amp;","&amp;K16&amp;","&amp;L16&amp;","&amp;M16&amp;","&amp;N16&amp;","&amp;O16&amp;","&amp;P16&amp;","&amp;","&amp;R16&amp;","&amp;S16&amp;","&amp;R16&amp;","&amp;T16&amp;","&amp;C18&amp;","&amp;D18&amp;","&amp;E18&amp;","&amp;G18&amp;","&amp;H18&amp;","&amp;I18&amp;","&amp;J18&amp;","&amp;K18&amp;","&amp;L18&amp;","&amp;M18&amp;","&amp;N18&amp;","&amp;O18&amp;","&amp;P18&amp;","&amp;Q18&amp;","&amp;R18&amp;","&amp;S18&amp;","&amp;D20&amp;","&amp;E20&amp;","&amp;F20&amp;","&amp;G20&amp;","&amp;H20&amp;","&amp;I20&amp;","&amp;J20&amp;","&amp;K20&amp;","&amp;L20&amp;","&amp;M20&amp;","&amp;N20&amp;","&amp;O20&amp;","&amp;P20&amp;","&amp;Q20&amp;","&amp;R20&amp;","&amp;S20&amp;","&amp;T20</f>
-        <v>22,23,24,25,26,27,28,29,30,31,32,33,34,35,36,37,38,61,62,63,65,66,67,68,69,70,71,72,73,74,75,76,77,102,103,104,105,106,107,108,109,110,111,112,113,114,116,117,118,142,143,144,145,146,147,148,149,150,151,152,153,154,155,156,157,181,182,184,185,186,187,188,189,190,191,192,193,194,195,197,198,201,202,204,205,206,207,208,209,210,211,212,213,214,215,217,218,242,243,244,245,246,247,248,249,250,251,252,253,254,255,256,257,282,283,284,285,286,287,288,289,290,291,292,293,294,,296,297,296,298,321,322,323,325,326,327,328,329,330,331,332,333,334,335,336,337,362,363,364,365,366,367,368,369,370,371,372,373,374,375,376,377,378</v>
-      </c>
-    </row>
-    <row r="3" spans="2:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="4">
-        <v>20</v>
-      </c>
-      <c r="C3" s="5">
-        <v>21</v>
-      </c>
-      <c r="D3" s="2">
-        <v>22</v>
-      </c>
-      <c r="E3" s="2">
-        <v>23</v>
-      </c>
-      <c r="F3" s="2">
-        <v>24</v>
-      </c>
-      <c r="G3" s="2">
-        <v>25</v>
-      </c>
-      <c r="H3" s="2">
-        <v>26</v>
-      </c>
-      <c r="I3" s="2">
-        <v>27</v>
-      </c>
-      <c r="J3" s="2">
-        <v>28</v>
-      </c>
-      <c r="K3" s="2">
-        <v>29</v>
-      </c>
-      <c r="L3" s="2">
-        <v>30</v>
-      </c>
-      <c r="M3" s="2">
-        <v>31</v>
-      </c>
-      <c r="N3" s="2">
-        <v>32</v>
-      </c>
-      <c r="O3" s="2">
-        <v>33</v>
-      </c>
-      <c r="P3" s="2">
-        <v>34</v>
-      </c>
-      <c r="Q3" s="2">
-        <v>35</v>
-      </c>
-      <c r="R3" s="2">
-        <v>36</v>
-      </c>
-      <c r="S3" s="2">
-        <v>37</v>
-      </c>
-      <c r="T3" s="2">
-        <v>38</v>
-      </c>
-      <c r="U3" s="4">
-        <v>39</v>
-      </c>
-      <c r="V3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="2:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="4">
-        <v>40</v>
-      </c>
-      <c r="C4" s="1">
-        <v>41</v>
-      </c>
-      <c r="D4" s="1">
-        <v>42</v>
-      </c>
-      <c r="E4" s="1">
-        <v>43</v>
-      </c>
-      <c r="F4" s="1">
-        <v>44</v>
-      </c>
-      <c r="G4" s="1">
-        <v>45</v>
-      </c>
-      <c r="H4" s="1">
-        <v>46</v>
-      </c>
-      <c r="I4" s="1">
-        <v>47</v>
-      </c>
-      <c r="J4" s="1">
-        <v>48</v>
-      </c>
-      <c r="K4" s="1">
-        <v>49</v>
-      </c>
-      <c r="L4" s="1">
-        <v>50</v>
-      </c>
-      <c r="M4" s="1">
-        <v>51</v>
-      </c>
-      <c r="N4" s="1">
-        <v>52</v>
-      </c>
-      <c r="O4" s="1">
-        <v>53</v>
-      </c>
-      <c r="P4" s="1">
-        <v>54</v>
-      </c>
-      <c r="Q4" s="1">
-        <v>55</v>
-      </c>
-      <c r="R4" s="1">
-        <v>56</v>
-      </c>
-      <c r="S4" s="1">
-        <v>57</v>
-      </c>
-      <c r="T4" s="1">
-        <v>58</v>
-      </c>
-      <c r="U4" s="4">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="2:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="4">
-        <v>60</v>
-      </c>
-      <c r="C5" s="2">
-        <v>61</v>
-      </c>
-      <c r="D5" s="2">
-        <v>62</v>
-      </c>
-      <c r="E5" s="2">
-        <v>63</v>
-      </c>
-      <c r="F5" s="1">
-        <v>64</v>
-      </c>
-      <c r="G5" s="2">
-        <v>65</v>
-      </c>
-      <c r="H5" s="2">
-        <v>66</v>
-      </c>
-      <c r="I5" s="2">
-        <v>67</v>
-      </c>
-      <c r="J5" s="2">
-        <v>68</v>
-      </c>
-      <c r="K5" s="2">
-        <v>69</v>
-      </c>
-      <c r="L5" s="2">
-        <v>70</v>
-      </c>
-      <c r="M5" s="2">
-        <v>71</v>
-      </c>
-      <c r="N5" s="2">
-        <v>72</v>
-      </c>
-      <c r="O5" s="2">
-        <v>73</v>
-      </c>
-      <c r="P5" s="2">
-        <v>74</v>
-      </c>
-      <c r="Q5" s="2">
-        <v>75</v>
-      </c>
-      <c r="R5" s="2">
-        <v>76</v>
-      </c>
-      <c r="S5" s="2">
-        <v>77</v>
-      </c>
-      <c r="T5" s="1">
-        <v>78</v>
-      </c>
-      <c r="U5" s="4">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="6" spans="2:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="4">
-        <v>80</v>
-      </c>
-      <c r="C6" s="1">
-        <v>81</v>
-      </c>
-      <c r="D6" s="1">
-        <v>82</v>
-      </c>
-      <c r="E6" s="1">
-        <v>83</v>
-      </c>
-      <c r="F6" s="1">
-        <v>84</v>
-      </c>
-      <c r="G6" s="1">
-        <v>85</v>
-      </c>
-      <c r="H6" s="1">
-        <v>86</v>
-      </c>
-      <c r="I6" s="1">
-        <v>87</v>
-      </c>
-      <c r="J6" s="1">
-        <v>88</v>
-      </c>
-      <c r="K6" s="1">
-        <v>89</v>
-      </c>
-      <c r="L6" s="1">
-        <v>90</v>
-      </c>
-      <c r="M6" s="1">
-        <v>91</v>
-      </c>
-      <c r="N6" s="1">
-        <v>92</v>
-      </c>
-      <c r="O6" s="1">
-        <v>93</v>
-      </c>
-      <c r="P6" s="1">
-        <v>94</v>
-      </c>
-      <c r="Q6" s="1">
-        <v>95</v>
-      </c>
-      <c r="R6" s="1">
-        <v>96</v>
-      </c>
-      <c r="S6" s="1">
-        <v>97</v>
-      </c>
-      <c r="T6" s="1">
-        <v>98</v>
-      </c>
-      <c r="U6" s="4">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="7" spans="2:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="4">
-        <v>100</v>
-      </c>
-      <c r="C7" s="1">
-        <v>101</v>
-      </c>
-      <c r="D7" s="2">
-        <v>102</v>
-      </c>
-      <c r="E7" s="2">
-        <v>103</v>
-      </c>
-      <c r="F7" s="2">
-        <v>104</v>
-      </c>
-      <c r="G7" s="2">
-        <v>105</v>
-      </c>
-      <c r="H7" s="2">
-        <v>106</v>
-      </c>
-      <c r="I7" s="2">
-        <v>107</v>
-      </c>
-      <c r="J7" s="2">
-        <v>108</v>
-      </c>
-      <c r="K7" s="2">
-        <v>109</v>
-      </c>
-      <c r="L7" s="2">
-        <v>110</v>
-      </c>
-      <c r="M7" s="2">
-        <v>111</v>
-      </c>
-      <c r="N7" s="2">
-        <v>112</v>
-      </c>
-      <c r="O7" s="2">
-        <v>113</v>
-      </c>
-      <c r="P7" s="2">
-        <v>114</v>
-      </c>
-      <c r="Q7" s="1">
-        <v>115</v>
-      </c>
-      <c r="R7" s="2">
-        <v>116</v>
-      </c>
-      <c r="S7" s="2">
-        <v>117</v>
-      </c>
-      <c r="T7" s="2">
-        <v>118</v>
-      </c>
-      <c r="U7" s="4">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="8" spans="2:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="4">
-        <v>120</v>
-      </c>
-      <c r="C8" s="1">
-        <v>121</v>
-      </c>
-      <c r="D8" s="1">
-        <v>122</v>
-      </c>
-      <c r="E8" s="1">
-        <v>123</v>
-      </c>
-      <c r="F8" s="1">
-        <v>124</v>
-      </c>
-      <c r="G8" s="1">
-        <v>125</v>
-      </c>
-      <c r="H8" s="1">
-        <v>126</v>
-      </c>
-      <c r="I8" s="1">
-        <v>127</v>
-      </c>
-      <c r="J8" s="1">
-        <v>128</v>
-      </c>
-      <c r="K8" s="1">
-        <v>129</v>
-      </c>
-      <c r="L8" s="1">
-        <v>130</v>
-      </c>
-      <c r="M8" s="1">
-        <v>131</v>
-      </c>
-      <c r="N8" s="1">
-        <v>132</v>
-      </c>
-      <c r="O8" s="1">
-        <v>133</v>
-      </c>
-      <c r="P8" s="1">
-        <v>134</v>
-      </c>
-      <c r="Q8" s="1">
-        <v>135</v>
-      </c>
-      <c r="R8" s="1">
-        <v>136</v>
-      </c>
-      <c r="S8" s="1">
-        <v>137</v>
-      </c>
-      <c r="T8" s="1">
-        <v>138</v>
-      </c>
-      <c r="U8" s="4">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="9" spans="2:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="4">
-        <v>140</v>
-      </c>
-      <c r="C9" s="1">
-        <v>141</v>
-      </c>
-      <c r="D9" s="2">
-        <v>142</v>
-      </c>
-      <c r="E9" s="2">
-        <v>143</v>
-      </c>
-      <c r="F9" s="2">
-        <v>144</v>
-      </c>
-      <c r="G9" s="2">
-        <v>145</v>
-      </c>
-      <c r="H9" s="2">
-        <v>146</v>
-      </c>
-      <c r="I9" s="2">
-        <v>147</v>
-      </c>
-      <c r="J9" s="2">
-        <v>148</v>
-      </c>
-      <c r="K9" s="2">
-        <v>149</v>
-      </c>
-      <c r="L9" s="2">
-        <v>150</v>
-      </c>
-      <c r="M9" s="2">
-        <v>151</v>
-      </c>
-      <c r="N9" s="2">
-        <v>152</v>
-      </c>
-      <c r="O9" s="2">
-        <v>153</v>
-      </c>
-      <c r="P9" s="2">
-        <v>154</v>
-      </c>
-      <c r="Q9" s="2">
-        <v>155</v>
-      </c>
-      <c r="R9" s="2">
-        <v>156</v>
-      </c>
-      <c r="S9" s="2">
-        <v>157</v>
-      </c>
-      <c r="T9" s="1">
-        <v>158</v>
-      </c>
-      <c r="U9" s="4">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="10" spans="2:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="4">
-        <v>160</v>
-      </c>
-      <c r="C10" s="1">
-        <v>161</v>
-      </c>
-      <c r="D10" s="1">
-        <v>162</v>
-      </c>
-      <c r="E10" s="1">
-        <v>163</v>
-      </c>
-      <c r="F10" s="1">
-        <v>164</v>
-      </c>
-      <c r="G10" s="1">
-        <v>165</v>
-      </c>
-      <c r="H10" s="1">
-        <v>166</v>
-      </c>
-      <c r="I10" s="1">
-        <v>167</v>
-      </c>
-      <c r="J10" s="1">
-        <v>168</v>
-      </c>
-      <c r="K10" s="1">
-        <v>169</v>
-      </c>
-      <c r="L10" s="1">
-        <v>170</v>
-      </c>
-      <c r="M10" s="1">
-        <v>171</v>
-      </c>
-      <c r="N10" s="1">
-        <v>172</v>
-      </c>
-      <c r="O10" s="1">
-        <v>173</v>
-      </c>
-      <c r="P10" s="1">
-        <v>174</v>
-      </c>
-      <c r="Q10" s="1">
-        <v>175</v>
-      </c>
-      <c r="R10" s="1">
-        <v>176</v>
-      </c>
-      <c r="S10" s="1">
-        <v>177</v>
-      </c>
-      <c r="T10" s="8">
-        <v>178</v>
-      </c>
-      <c r="U10" s="4">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="11" spans="2:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="4">
-        <v>180</v>
-      </c>
-      <c r="C11" s="2">
-        <v>181</v>
-      </c>
-      <c r="D11" s="2">
-        <v>182</v>
-      </c>
-      <c r="E11" s="1">
-        <v>183</v>
-      </c>
-      <c r="F11" s="2">
-        <v>184</v>
-      </c>
-      <c r="G11" s="2">
-        <v>185</v>
-      </c>
-      <c r="H11" s="2">
-        <v>186</v>
-      </c>
-      <c r="I11" s="2">
-        <v>187</v>
-      </c>
-      <c r="J11" s="2">
-        <v>188</v>
-      </c>
-      <c r="K11" s="2">
-        <v>189</v>
-      </c>
-      <c r="L11" s="2">
-        <v>190</v>
-      </c>
-      <c r="M11" s="2">
-        <v>191</v>
-      </c>
-      <c r="N11" s="2">
-        <v>192</v>
-      </c>
-      <c r="O11" s="2">
-        <v>193</v>
-      </c>
-      <c r="P11" s="2">
-        <v>194</v>
-      </c>
-      <c r="Q11" s="2">
-        <v>195</v>
-      </c>
-      <c r="R11" s="1">
-        <v>196</v>
-      </c>
-      <c r="S11" s="2">
-        <v>197</v>
-      </c>
-      <c r="T11" s="2">
-        <v>198</v>
-      </c>
-      <c r="U11" s="4">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="12" spans="2:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="4">
-        <v>200</v>
-      </c>
-      <c r="C12" s="2">
-        <v>201</v>
-      </c>
-      <c r="D12" s="2">
-        <v>202</v>
-      </c>
-      <c r="E12" s="1">
-        <v>203</v>
-      </c>
-      <c r="F12" s="2">
-        <v>204</v>
-      </c>
-      <c r="G12" s="2">
-        <v>205</v>
-      </c>
-      <c r="H12" s="2">
-        <v>206</v>
-      </c>
-      <c r="I12" s="2">
-        <v>207</v>
-      </c>
-      <c r="J12" s="2">
-        <v>208</v>
-      </c>
-      <c r="K12" s="2">
-        <v>209</v>
-      </c>
-      <c r="L12" s="2">
-        <v>210</v>
-      </c>
-      <c r="M12" s="2">
-        <v>211</v>
-      </c>
-      <c r="N12" s="2">
-        <v>212</v>
-      </c>
-      <c r="O12" s="2">
-        <v>213</v>
-      </c>
-      <c r="P12" s="2">
-        <v>214</v>
-      </c>
-      <c r="Q12" s="2">
-        <v>215</v>
-      </c>
-      <c r="R12" s="1">
-        <v>216</v>
-      </c>
-      <c r="S12" s="2">
-        <v>217</v>
-      </c>
-      <c r="T12" s="2">
-        <v>218</v>
-      </c>
-      <c r="U12" s="4">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="13" spans="2:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="4">
-        <v>220</v>
-      </c>
-      <c r="C13" s="7">
-        <v>221</v>
-      </c>
-      <c r="D13" s="1">
-        <v>222</v>
-      </c>
-      <c r="E13" s="1">
-        <v>223</v>
-      </c>
-      <c r="F13" s="1">
-        <v>224</v>
-      </c>
-      <c r="G13" s="1">
-        <v>225</v>
-      </c>
-      <c r="H13" s="1">
-        <v>226</v>
-      </c>
-      <c r="I13" s="1">
-        <v>227</v>
-      </c>
-      <c r="J13" s="1">
-        <v>228</v>
-      </c>
-      <c r="K13" s="1">
-        <v>229</v>
-      </c>
-      <c r="L13" s="1">
-        <v>230</v>
-      </c>
-      <c r="M13" s="1">
-        <v>231</v>
-      </c>
-      <c r="N13" s="1">
-        <v>232</v>
-      </c>
-      <c r="O13" s="1">
-        <v>233</v>
-      </c>
-      <c r="P13" s="1">
-        <v>234</v>
-      </c>
-      <c r="Q13" s="1">
-        <v>235</v>
-      </c>
-      <c r="R13" s="1">
-        <v>236</v>
-      </c>
-      <c r="S13" s="1">
-        <v>237</v>
-      </c>
-      <c r="T13" s="1">
-        <v>238</v>
-      </c>
-      <c r="U13" s="4">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="14" spans="2:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="4">
-        <v>240</v>
-      </c>
-      <c r="C14" s="1">
-        <v>241</v>
-      </c>
-      <c r="D14" s="2">
-        <v>242</v>
-      </c>
-      <c r="E14" s="2">
-        <v>243</v>
-      </c>
-      <c r="F14" s="2">
-        <v>244</v>
-      </c>
-      <c r="G14" s="2">
-        <v>245</v>
-      </c>
-      <c r="H14" s="2">
-        <v>246</v>
-      </c>
-      <c r="I14" s="2">
-        <v>247</v>
-      </c>
-      <c r="J14" s="2">
-        <v>248</v>
-      </c>
-      <c r="K14" s="2">
-        <v>249</v>
-      </c>
-      <c r="L14" s="2">
-        <v>250</v>
-      </c>
-      <c r="M14" s="2">
-        <v>251</v>
-      </c>
-      <c r="N14" s="2">
-        <v>252</v>
-      </c>
-      <c r="O14" s="2">
-        <v>253</v>
-      </c>
-      <c r="P14" s="2">
-        <v>254</v>
-      </c>
-      <c r="Q14" s="2">
-        <v>255</v>
-      </c>
-      <c r="R14" s="2">
-        <v>256</v>
-      </c>
-      <c r="S14" s="2">
-        <v>257</v>
-      </c>
-      <c r="T14" s="1">
-        <v>258</v>
-      </c>
-      <c r="U14" s="4">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="15" spans="2:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="4">
-        <v>260</v>
-      </c>
-      <c r="C15" s="1">
-        <v>261</v>
-      </c>
-      <c r="D15" s="1">
-        <v>262</v>
-      </c>
-      <c r="E15" s="1">
-        <v>263</v>
-      </c>
-      <c r="F15" s="1">
-        <v>264</v>
-      </c>
-      <c r="G15" s="1">
-        <v>265</v>
-      </c>
-      <c r="H15" s="1">
-        <v>266</v>
-      </c>
-      <c r="I15" s="1">
-        <v>267</v>
-      </c>
-      <c r="J15" s="1">
-        <v>268</v>
-      </c>
-      <c r="K15" s="1">
-        <v>269</v>
-      </c>
-      <c r="L15" s="1">
-        <v>270</v>
-      </c>
-      <c r="M15" s="1">
-        <v>271</v>
-      </c>
-      <c r="N15" s="1">
-        <v>272</v>
-      </c>
-      <c r="O15" s="1">
-        <v>273</v>
-      </c>
-      <c r="P15" s="1">
-        <v>274</v>
-      </c>
-      <c r="Q15" s="1">
-        <v>275</v>
-      </c>
-      <c r="R15" s="1">
-        <v>276</v>
-      </c>
-      <c r="S15" s="1">
-        <v>277</v>
-      </c>
-      <c r="T15" s="9">
-        <v>278</v>
-      </c>
-      <c r="U15" s="4">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="16" spans="2:22" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="4">
-        <v>280</v>
-      </c>
-      <c r="C16" s="1">
-        <v>281</v>
-      </c>
-      <c r="D16" s="2">
-        <v>282</v>
-      </c>
-      <c r="E16" s="2">
-        <v>283</v>
-      </c>
-      <c r="F16" s="2">
-        <v>284</v>
-      </c>
-      <c r="G16" s="2">
-        <v>285</v>
-      </c>
-      <c r="H16" s="2">
-        <v>286</v>
-      </c>
-      <c r="I16" s="2">
-        <v>287</v>
-      </c>
-      <c r="J16" s="2">
-        <v>288</v>
-      </c>
-      <c r="K16" s="2">
-        <v>289</v>
-      </c>
-      <c r="L16" s="2">
-        <v>290</v>
-      </c>
-      <c r="M16" s="2">
-        <v>291</v>
-      </c>
-      <c r="N16" s="2">
-        <v>292</v>
-      </c>
-      <c r="O16" s="2">
-        <v>293</v>
-      </c>
-      <c r="P16" s="2">
-        <v>294</v>
-      </c>
-      <c r="Q16" s="1">
-        <v>295</v>
-      </c>
-      <c r="R16" s="2">
-        <v>296</v>
-      </c>
-      <c r="S16" s="2">
-        <v>297</v>
-      </c>
-      <c r="T16" s="2">
-        <v>298</v>
-      </c>
-      <c r="U16" s="4">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="17" spans="2:21" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="4">
-        <v>300</v>
-      </c>
-      <c r="C17" s="1">
-        <v>301</v>
-      </c>
-      <c r="D17" s="1">
-        <v>302</v>
-      </c>
-      <c r="E17" s="1">
-        <v>303</v>
-      </c>
-      <c r="F17" s="1">
-        <v>304</v>
-      </c>
-      <c r="G17" s="1">
-        <v>305</v>
-      </c>
-      <c r="H17" s="1">
-        <v>306</v>
-      </c>
-      <c r="I17" s="1">
-        <v>307</v>
-      </c>
-      <c r="J17" s="1">
-        <v>308</v>
-      </c>
-      <c r="K17" s="1">
-        <v>309</v>
-      </c>
-      <c r="L17" s="1">
-        <v>310</v>
-      </c>
-      <c r="M17" s="1">
-        <v>311</v>
-      </c>
-      <c r="N17" s="1">
-        <v>312</v>
-      </c>
-      <c r="O17" s="1">
-        <v>313</v>
-      </c>
-      <c r="P17" s="1">
-        <v>314</v>
-      </c>
-      <c r="Q17" s="1">
-        <v>315</v>
-      </c>
-      <c r="R17" s="1">
-        <v>316</v>
-      </c>
-      <c r="S17" s="1">
-        <v>317</v>
-      </c>
-      <c r="T17" s="1">
-        <v>318</v>
-      </c>
-      <c r="U17" s="4">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="18" spans="2:21" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="4">
-        <v>320</v>
-      </c>
-      <c r="C18" s="2">
-        <v>321</v>
-      </c>
-      <c r="D18" s="2">
-        <v>322</v>
-      </c>
-      <c r="E18" s="2">
-        <v>323</v>
-      </c>
-      <c r="F18" s="1">
-        <v>324</v>
-      </c>
-      <c r="G18" s="2">
-        <v>325</v>
-      </c>
-      <c r="H18" s="2">
-        <v>326</v>
-      </c>
-      <c r="I18" s="2">
-        <v>327</v>
-      </c>
-      <c r="J18" s="2">
-        <v>328</v>
-      </c>
-      <c r="K18" s="2">
-        <v>329</v>
-      </c>
-      <c r="L18" s="2">
-        <v>330</v>
-      </c>
-      <c r="M18" s="2">
-        <v>331</v>
-      </c>
-      <c r="N18" s="2">
-        <v>332</v>
-      </c>
-      <c r="O18" s="2">
-        <v>333</v>
-      </c>
-      <c r="P18" s="2">
-        <v>334</v>
-      </c>
-      <c r="Q18" s="2">
-        <v>335</v>
-      </c>
-      <c r="R18" s="2">
-        <v>336</v>
-      </c>
-      <c r="S18" s="2">
-        <v>337</v>
-      </c>
-      <c r="T18" s="1">
-        <v>338</v>
-      </c>
-      <c r="U18" s="4">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="19" spans="2:21" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="4">
-        <v>340</v>
-      </c>
-      <c r="C19" s="1">
-        <v>341</v>
-      </c>
-      <c r="D19" s="1">
-        <v>342</v>
-      </c>
-      <c r="E19" s="1">
-        <v>343</v>
-      </c>
-      <c r="F19" s="1">
-        <v>344</v>
-      </c>
-      <c r="G19" s="1">
-        <v>345</v>
-      </c>
-      <c r="H19" s="1">
-        <v>346</v>
-      </c>
-      <c r="I19" s="1">
-        <v>347</v>
-      </c>
-      <c r="J19" s="1">
-        <v>348</v>
-      </c>
-      <c r="K19" s="1">
-        <v>349</v>
-      </c>
-      <c r="L19" s="1">
-        <v>350</v>
-      </c>
-      <c r="M19" s="1">
-        <v>351</v>
-      </c>
-      <c r="N19" s="1">
-        <v>352</v>
-      </c>
-      <c r="O19" s="1">
-        <v>353</v>
-      </c>
-      <c r="P19" s="1">
-        <v>354</v>
-      </c>
-      <c r="Q19" s="1">
-        <v>355</v>
-      </c>
-      <c r="R19" s="1">
-        <v>356</v>
-      </c>
-      <c r="S19" s="1">
-        <v>357</v>
-      </c>
-      <c r="T19" s="1">
-        <v>358</v>
-      </c>
-      <c r="U19" s="4">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="20" spans="2:21" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="4">
-        <v>360</v>
-      </c>
-      <c r="C20" s="6">
-        <v>361</v>
-      </c>
-      <c r="D20" s="2">
-        <v>362</v>
-      </c>
-      <c r="E20" s="2">
-        <v>363</v>
-      </c>
-      <c r="F20" s="2">
-        <v>364</v>
-      </c>
-      <c r="G20" s="2">
-        <v>365</v>
-      </c>
-      <c r="H20" s="2">
-        <v>366</v>
-      </c>
-      <c r="I20" s="2">
-        <v>367</v>
-      </c>
-      <c r="J20" s="2">
-        <v>368</v>
-      </c>
-      <c r="K20" s="2">
-        <v>369</v>
-      </c>
-      <c r="L20" s="2">
-        <v>370</v>
-      </c>
-      <c r="M20" s="2">
-        <v>371</v>
-      </c>
-      <c r="N20" s="2">
-        <v>372</v>
-      </c>
-      <c r="O20" s="2">
-        <v>373</v>
-      </c>
-      <c r="P20" s="2">
-        <v>374</v>
-      </c>
-      <c r="Q20" s="2">
-        <v>375</v>
-      </c>
-      <c r="R20" s="2">
-        <v>376</v>
-      </c>
-      <c r="S20" s="2">
-        <v>377</v>
-      </c>
-      <c r="T20" s="2">
-        <v>378</v>
-      </c>
-      <c r="U20" s="4">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="21" spans="2:21" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="4">
-        <v>380</v>
-      </c>
-      <c r="C21" s="4">
-        <v>381</v>
-      </c>
-      <c r="D21" s="4">
-        <v>382</v>
-      </c>
-      <c r="E21" s="4">
-        <v>383</v>
-      </c>
-      <c r="F21" s="4">
-        <v>384</v>
-      </c>
-      <c r="G21" s="4">
-        <v>385</v>
-      </c>
-      <c r="H21" s="4">
-        <v>386</v>
-      </c>
-      <c r="I21" s="4">
-        <v>387</v>
-      </c>
-      <c r="J21" s="4">
-        <v>388</v>
-      </c>
-      <c r="K21" s="4">
-        <v>389</v>
-      </c>
-      <c r="L21" s="4">
-        <v>390</v>
-      </c>
-      <c r="M21" s="4">
-        <v>391</v>
-      </c>
-      <c r="N21" s="4">
-        <v>392</v>
-      </c>
-      <c r="O21" s="4">
-        <v>393</v>
-      </c>
-      <c r="P21" s="4">
-        <v>394</v>
-      </c>
-      <c r="Q21" s="4">
-        <v>395</v>
-      </c>
-      <c r="R21" s="4">
-        <v>396</v>
-      </c>
-      <c r="S21" s="4">
-        <v>397</v>
-      </c>
-      <c r="T21" s="4">
-        <v>398</v>
-      </c>
-      <c r="U21" s="4">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="22" spans="2:21" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="G22" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="H22" s="9" t="s">
-        <v>3</v>
-      </c>
+      <c r="I22" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
working with lots of bugs
</commit_message>
<xml_diff>
--- a/pacman-wall-mapping.xlsx
+++ b/pacman-wall-mapping.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wesleyhall/development/PROJECTS/wdi-project-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC9D7BB-9C13-6447-9F8A-E4C946967011}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83B7C2B2-1DF7-1B43-A390-AA75C2E0B890}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="24260" windowHeight="20540" activeTab="4" xr2:uid="{1EA259AE-86C8-2D4F-8109-A100E6DB6DF0}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24260" windowHeight="20540" xr2:uid="{1EA259AE-86C8-2D4F-8109-A100E6DB6DF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Level 1" sheetId="1" r:id="rId1"/>
@@ -498,7 +498,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{888E5F92-0FDF-8647-8DCE-E19EF0F1C882}">
   <dimension ref="B1:U22"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
@@ -1770,7 +1770,9 @@
       <c r="H22" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="I22" s="10"/>
+      <c r="I22" s="10">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5648,7 +5650,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B86CBA31-09A1-CF47-B6B2-15E4927C6684}">
   <dimension ref="B1:V22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>